<commit_message>
Working on assembly reference classes in source generator and authorization
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -33,30 +33,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>EditRoles</t>
-  </si>
-  <si>
-    <t>ReadRoles</t>
-  </si>
-  <si>
-    <t>InsertRoles</t>
-  </si>
-  <si>
-    <t>DeleteRoles</t>
-  </si>
-  <si>
-    <t>ReadUsers</t>
-  </si>
-  <si>
-    <t>EditUsers</t>
-  </si>
-  <si>
-    <t>InsertUsers</t>
-  </si>
-  <si>
-    <t>DeleteUsers</t>
-  </si>
-  <si>
     <t>Read roles</t>
   </si>
   <si>
@@ -112,6 +88,30 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>ReadRole</t>
+  </si>
+  <si>
+    <t>EditRole</t>
+  </si>
+  <si>
+    <t>InsertRole</t>
+  </si>
+  <si>
+    <t>DeleteRole</t>
+  </si>
+  <si>
+    <t>ReadUserExtended</t>
+  </si>
+  <si>
+    <t>EditUserExtended</t>
+  </si>
+  <si>
+    <t>InsertUserExtended</t>
+  </si>
+  <si>
+    <t>DeleteUserExtended</t>
   </si>
 </sst>
 </file>
@@ -215,7 +215,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -227,16 +227,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="7"/>
     <cellStyle name="Hyperlink" xfId="2"/>
-    <cellStyle name="Hyperlink" xfId="11"/>
     <cellStyle name="Hyperlink 2" xfId="8"/>
     <cellStyle name="Neutral 2" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +550,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -573,25 +571,29 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
+        <v>delete from Permissions; dbcc checkident (Permissions, reseed, 0);</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -599,17 +601,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="H3" t="str">
-        <f>CONCATENATE("insert into ",$A$1,"(",$A$2,",",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(",A3,", N'",B3,"', N'",C3,"', ",IF(TRIM(D3)&lt;&gt;"","N'"&amp;D3&amp;"'","null"),", ",IF(TRIM(E3)&lt;&gt;"","N'"&amp;E3&amp;"'","null")," , ",IF(TRIM(F3)&lt;&gt;"","N'"&amp;F3&amp;"'","null"),", N'",G3,"');")</f>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(1, N'Read roles', N'Vidi uloge', null, null , null, N'ReadRoles');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B3,"', N'",C3,"', ",IF(TRIM(D3)&lt;&gt;"","N'"&amp;D3&amp;"'","null"),", ",IF(TRIM(E3)&lt;&gt;"","N'"&amp;E3&amp;"'","null")," , getdate(), N'",G3,"');")</f>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read roles', N'Vidi uloge', null, null , getdate(), N'ReadRole');</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -617,17 +619,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" ref="H4:H10" si="0">CONCATENATE("insert into ",$A$1,"(",$A$2,",",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(",A4,", N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , ",IF(TRIM(F4)&lt;&gt;"","N'"&amp;F4&amp;"'","null"),", N'",G4,"');")</f>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(2, N'Edit roles', N'Promeni uloge', null, null , null, N'EditRoles');</v>
+        <f t="shared" ref="H4:H10" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , getdate(), N'",G4,"');")</f>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit roles', N'Promeni uloge', null, null , getdate(), N'EditRole');</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -635,17 +637,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(3, N'Insert roles', N'Dodaj uloge', null, null , null, N'InsertRoles');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert roles', N'Dodaj uloge', null, null , getdate(), N'InsertRole');</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -653,17 +655,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="H6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(4, N'Delete roles', N'Obriši uloge', null, null , null, N'DeleteRoles');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete roles', N'Obriši uloge', null, null , getdate(), N'DeleteRole');</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -671,17 +673,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(5, N'Read users', N'Vidi korisnike', null, null , null, N'ReadUsers');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read users', N'Vidi korisnike', null, null , getdate(), N'ReadUserExtended');</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -689,17 +691,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(6, N'Edit users', N'Promeni korisnike', null, null , null, N'EditUsers');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit users', N'Promeni korisnike', null, null , getdate(), N'EditUserExtended');</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -707,17 +709,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(7, N'Insert users', N'Dodaj korisnike', null, null , null, N'InsertUsers');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert users', N'Dodaj korisnike', null, null , getdate(), N'InsertUserExtended');</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -725,21 +727,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="H10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Id,Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(8, N'Delete users', N'Obriši korisnike', null, null , null, N'DeleteUsers');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete users', N'Obriši korisnike', null, null , getdate(), N'DeleteUserExtended');</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Business logic and fixing bugs in source generator.
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
     <sheet name="Permissions" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TransactionStatuses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Permissions</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Edit users</t>
   </si>
   <si>
-    <t>Insert users</t>
-  </si>
-  <si>
     <t>Delete users</t>
   </si>
   <si>
@@ -63,30 +60,6 @@
     <t>DescriptionLatin</t>
   </si>
   <si>
-    <t>Vidi uloge</t>
-  </si>
-  <si>
-    <t>Promeni uloge</t>
-  </si>
-  <si>
-    <t>Dodaj uloge</t>
-  </si>
-  <si>
-    <t>Obriši uloge</t>
-  </si>
-  <si>
-    <t>Vidi korisnike</t>
-  </si>
-  <si>
-    <t>Promeni korisnike</t>
-  </si>
-  <si>
-    <t>Dodaj korisnike</t>
-  </si>
-  <si>
-    <t>Obriši korisnike</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -108,10 +81,112 @@
     <t>EditUserExtended</t>
   </si>
   <si>
-    <t>InsertUserExtended</t>
-  </si>
-  <si>
     <t>DeleteUserExtended</t>
+  </si>
+  <si>
+    <t>TransactionStatuses</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Kompletirana</t>
+  </si>
+  <si>
+    <t>Otkazana</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Read permissions</t>
+  </si>
+  <si>
+    <t>Read tiers</t>
+  </si>
+  <si>
+    <t>Edit tiers</t>
+  </si>
+  <si>
+    <t>Insert tiers</t>
+  </si>
+  <si>
+    <t>Delete tiers</t>
+  </si>
+  <si>
+    <t>Pregled uloga korisnika</t>
+  </si>
+  <si>
+    <t>Promena uloga korisnika</t>
+  </si>
+  <si>
+    <t>Promena nivoa odanosti</t>
+  </si>
+  <si>
+    <t>Dodavanje uloga korisnika</t>
+  </si>
+  <si>
+    <t>Promena profila korisnika</t>
+  </si>
+  <si>
+    <t>Pregled profila korisnika</t>
+  </si>
+  <si>
+    <t>Brisanje profila korisnika</t>
+  </si>
+  <si>
+    <t>Pregled permisija uloga</t>
+  </si>
+  <si>
+    <t>Pregled nivoa odanosti</t>
+  </si>
+  <si>
+    <t>Dodavanje nivoa odanosti</t>
+  </si>
+  <si>
+    <t>Brisanje nivoa odanosti</t>
+  </si>
+  <si>
+    <t>Brisanje uloga korisnika</t>
+  </si>
+  <si>
+    <t>Read transactions</t>
+  </si>
+  <si>
+    <t>Pregled transakcija</t>
+  </si>
+  <si>
+    <t>Read transaction products</t>
+  </si>
+  <si>
+    <t>Pregled proizvoda iz transakcije</t>
+  </si>
+  <si>
+    <t>Read transaction statuses</t>
+  </si>
+  <si>
+    <t>Pregled statusa transakcije</t>
+  </si>
+  <si>
+    <t>ReadPermission</t>
+  </si>
+  <si>
+    <t>InsertTier</t>
+  </si>
+  <si>
+    <t>ReadTier</t>
+  </si>
+  <si>
+    <t>EditTier</t>
+  </si>
+  <si>
+    <t>DeleteTier</t>
+  </si>
+  <si>
+    <t>ReadTransaction</t>
+  </si>
+  <si>
+    <t>ReadTransactionProduct</t>
   </si>
 </sst>
 </file>
@@ -547,17 +622,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
     <col min="4" max="4" width="51.85546875" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
@@ -570,20 +645,20 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>23</v>
+      <c r="A2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -603,142 +678,291 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B3,"', N'",C3,"', ",IF(TRIM(D3)&lt;&gt;"","N'"&amp;D3&amp;"'","null"),", ",IF(TRIM(E3)&lt;&gt;"","N'"&amp;E3&amp;"'","null")," , getdate(), N'",G3,"');")</f>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read roles', N'Vidi uloge', null, null , getdate(), N'ReadRole');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read roles', N'Pregled uloga korisnika', null, null , getdate(), N'ReadRole');</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" ref="H4:H10" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , getdate(), N'",G4,"');")</f>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit roles', N'Promeni uloge', null, null , getdate(), N'EditRole');</v>
+        <f t="shared" ref="H4:H17" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , getdate(), N'",G4,"');")</f>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit roles', N'Promena uloga korisnika', null, null , getdate(), N'EditRole');</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert roles', N'Dodaj uloge', null, null , getdate(), N'InsertRole');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert roles', N'Dodavanje uloga korisnika', null, null , getdate(), N'InsertRole');</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete roles', N'Obriši uloge', null, null , getdate(), N'DeleteRole');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete roles', N'Brisanje uloga korisnika', null, null , getdate(), N'DeleteRole');</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="H7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read users', N'Vidi korisnike', null, null , getdate(), N'ReadUserExtended');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read users', N'Pregled profila korisnika', null, null , getdate(), N'ReadUserExtended');</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit users', N'Promeni korisnike', null, null , getdate(), N'EditUserExtended');</v>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit users', N'Promena profila korisnika', null, null , getdate(), N'EditUserExtended');</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete users', N'Brisanje profila korisnika', null, null , getdate(), N'DeleteUserExtended');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read permissions', N'Pregled permisija uloga', null, null , getdate(), N'ReadPermission');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read tiers', N'Pregled nivoa odanosti', null, null , getdate(), N'ReadTier');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit tiers', N'Promena nivoa odanosti', null, null , getdate(), N'EditTier');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert users', N'Dodaj korisnike', null, null , getdate(), N'InsertUserExtended');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert tiers', N'Dodavanje nivoa odanosti', null, null , getdate(), N'InsertTier');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete users', N'Obriši korisnike', null, null , getdate(), N'DeleteUserExtended');</v>
-      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete tiers', N'Brisanje nivoa odanosti', null, null , getdate(), N'DeleteTier');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transactions', N'Pregled transakcija', null, null , getdate(), N'ReadTransaction');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transaction products', N'Pregled proizvoda iz transakcije', null, null , getdate(), N'ReadTransactionProduct');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -748,12 +972,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
+        <v>delete from TransactionStatuses; dbcc checkident (TransactionStatuses, reseed, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', N'",C3,"', N'",D3,"');")</f>
+        <v>insert into TransactionStatuses(Name, NameLatin, Code) values(N'Completed', N'Kompletirana', N'Completed');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', N'",C4,"', N'",D4,"');")</f>
+        <v>insert into TransactionStatuses(Name, NameLatin, Code) values(N'Cancelled', N'Otkazana', N'Cancelled');</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on the dashboard UI, tiers and notifications.
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Permissions</t>
   </si>
@@ -187,6 +187,45 @@
   </si>
   <si>
     <t>ReadTransactionProduct</t>
+  </si>
+  <si>
+    <t>ReadTransactionStatus</t>
+  </si>
+  <si>
+    <t>Read notifications</t>
+  </si>
+  <si>
+    <t>Edit notifications</t>
+  </si>
+  <si>
+    <t>Insert notifications</t>
+  </si>
+  <si>
+    <t>Delete notifications</t>
+  </si>
+  <si>
+    <t>Pregled notifikacija</t>
+  </si>
+  <si>
+    <t>Promena notifikacija</t>
+  </si>
+  <si>
+    <t>Dodavanje notifikacija</t>
+  </si>
+  <si>
+    <t>Brisanje notifikacija</t>
+  </si>
+  <si>
+    <t>ReadNotification</t>
+  </si>
+  <si>
+    <t>EditNotification</t>
+  </si>
+  <si>
+    <t>InsertNotification</t>
+  </si>
+  <si>
+    <t>DeleteNotification</t>
   </si>
 </sst>
 </file>
@@ -625,7 +664,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -703,7 +742,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" ref="H4:H17" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , getdate(), N'",G4,"');")</f>
+        <f t="shared" ref="H4:H21" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , getdate(), N'",G4,"');")</f>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit roles', N'Promena uloga korisnika', null, null , getdate(), N'EditRole');</v>
       </c>
     </row>
@@ -810,7 +849,7 @@
       <c r="G10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read permissions', N'Pregled permisija uloga', null, null , getdate(), N'ReadPermission');</v>
       </c>
@@ -828,7 +867,7 @@
       <c r="G11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read tiers', N'Pregled nivoa odanosti', null, null , getdate(), N'ReadTier');</v>
       </c>
@@ -846,7 +885,7 @@
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit tiers', N'Promena nivoa odanosti', null, null , getdate(), N'EditTier');</v>
       </c>
@@ -864,7 +903,7 @@
       <c r="G13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert tiers', N'Dodavanje nivoa odanosti', null, null , getdate(), N'InsertTier');</v>
       </c>
@@ -882,7 +921,7 @@
       <c r="G14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete tiers', N'Brisanje nivoa odanosti', null, null , getdate(), N'DeleteTier');</v>
       </c>
@@ -900,7 +939,7 @@
       <c r="G15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transactions', N'Pregled transakcija', null, null , getdate(), N'ReadTransaction');</v>
       </c>
@@ -918,12 +957,12 @@
       <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H16" t="str">
+      <c r="H16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transaction products', N'Pregled proizvoda iz transakcije', null, null , getdate(), N'ReadTransactionProduct');</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -933,33 +972,104 @@
       <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="G17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transaction statuses', N'Pregled statusa transakcije', null, null , getdate(), N'ReadTransactionStatus');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read notifications', N'Pregled notifikacija', null, null , getdate(), N'ReadNotification');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit notifications', N'Promena notifikacija', null, null , getdate(), N'EditNotification');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert notifications', N'Dodavanje notifikacija', null, null , getdate(), N'InsertNotification');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete notifications', N'Brisanje notifikacija', null, null , getdate(), N'DeleteNotification');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Working on the model, making discriminator for partner integration.
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -10,13 +10,16 @@
     <sheet name="Home" sheetId="1" r:id="rId1"/>
     <sheet name="Permissions" sheetId="2" r:id="rId2"/>
     <sheet name="TransactionStatuses" sheetId="3" r:id="rId3"/>
+    <sheet name="Genders" sheetId="4" r:id="rId4"/>
+    <sheet name="Municipalities" sheetId="5" r:id="rId5"/>
+    <sheet name="Companies" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="251">
   <si>
     <t>Permissions</t>
   </si>
@@ -226,6 +229,549 @@
   </si>
   <si>
     <t>DeleteNotification</t>
+  </si>
+  <si>
+    <t>Genders</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Muški</t>
+  </si>
+  <si>
+    <t>Ženski</t>
+  </si>
+  <si>
+    <t>Municipalities</t>
+  </si>
+  <si>
+    <t>Ada</t>
+  </si>
+  <si>
+    <t>Aleksandrovac</t>
+  </si>
+  <si>
+    <t>Aleksinac</t>
+  </si>
+  <si>
+    <t>Alibunar</t>
+  </si>
+  <si>
+    <t>Apatin</t>
+  </si>
+  <si>
+    <t>Aranđelovac</t>
+  </si>
+  <si>
+    <t>Arilje</t>
+  </si>
+  <si>
+    <t>Babušnica</t>
+  </si>
+  <si>
+    <t>Bajina Bašta</t>
+  </si>
+  <si>
+    <t>Batočina</t>
+  </si>
+  <si>
+    <t>Bač</t>
+  </si>
+  <si>
+    <t>Bačka Palanka</t>
+  </si>
+  <si>
+    <t>Bačka Topola</t>
+  </si>
+  <si>
+    <t>Bački Petrovac</t>
+  </si>
+  <si>
+    <t>Bela Palanka</t>
+  </si>
+  <si>
+    <t>Bela Crkva</t>
+  </si>
+  <si>
+    <t>Beograd - grad</t>
+  </si>
+  <si>
+    <t>Beočin</t>
+  </si>
+  <si>
+    <t>Bečej</t>
+  </si>
+  <si>
+    <t>Blace</t>
+  </si>
+  <si>
+    <t>Bogatić</t>
+  </si>
+  <si>
+    <t>Bojnik</t>
+  </si>
+  <si>
+    <t>Boljevac</t>
+  </si>
+  <si>
+    <t>Bor</t>
+  </si>
+  <si>
+    <t>Bosilegrad</t>
+  </si>
+  <si>
+    <t>Brus</t>
+  </si>
+  <si>
+    <t>Bujanovac</t>
+  </si>
+  <si>
+    <t>Valjevo - grad</t>
+  </si>
+  <si>
+    <t>Varvarin</t>
+  </si>
+  <si>
+    <t>Velika Plana</t>
+  </si>
+  <si>
+    <t>Veliko Gradište</t>
+  </si>
+  <si>
+    <t>Vladimirci</t>
+  </si>
+  <si>
+    <t>Vladičin Han</t>
+  </si>
+  <si>
+    <t>Vlasotince</t>
+  </si>
+  <si>
+    <t>Vranje - grad</t>
+  </si>
+  <si>
+    <t>Vrbas</t>
+  </si>
+  <si>
+    <t>Vrnjačka Banja</t>
+  </si>
+  <si>
+    <t>Vršac - grad</t>
+  </si>
+  <si>
+    <t>Gadžin Han</t>
+  </si>
+  <si>
+    <t>Golubac</t>
+  </si>
+  <si>
+    <t>Gornji Milanovac</t>
+  </si>
+  <si>
+    <t>Despotovac</t>
+  </si>
+  <si>
+    <t>Dimitrovgrad</t>
+  </si>
+  <si>
+    <t>Doljevac</t>
+  </si>
+  <si>
+    <t>Žabalj</t>
+  </si>
+  <si>
+    <t>Žabari</t>
+  </si>
+  <si>
+    <t>Žagubica</t>
+  </si>
+  <si>
+    <t>Žitište</t>
+  </si>
+  <si>
+    <t>Žitorađa</t>
+  </si>
+  <si>
+    <t>Zaječar - grad</t>
+  </si>
+  <si>
+    <t>Zrenjanin - grad</t>
+  </si>
+  <si>
+    <t>Ivanjica</t>
+  </si>
+  <si>
+    <t>Inđija</t>
+  </si>
+  <si>
+    <t>Irig</t>
+  </si>
+  <si>
+    <t>Jagodina - grad</t>
+  </si>
+  <si>
+    <t>Kanjiža</t>
+  </si>
+  <si>
+    <t>Kikinda - grad</t>
+  </si>
+  <si>
+    <t>Kladovo</t>
+  </si>
+  <si>
+    <t>Knić</t>
+  </si>
+  <si>
+    <t>Knjaževac</t>
+  </si>
+  <si>
+    <t>Kovačica</t>
+  </si>
+  <si>
+    <t>Kovin</t>
+  </si>
+  <si>
+    <t>Kosjerić</t>
+  </si>
+  <si>
+    <t>Koceljeva</t>
+  </si>
+  <si>
+    <t>Kragujevac - grad</t>
+  </si>
+  <si>
+    <t>Kraljevo - grad</t>
+  </si>
+  <si>
+    <t>Krupanj</t>
+  </si>
+  <si>
+    <t>Kruševac - grad</t>
+  </si>
+  <si>
+    <t>Kula</t>
+  </si>
+  <si>
+    <t>Kuršumlija</t>
+  </si>
+  <si>
+    <t>Kučevo</t>
+  </si>
+  <si>
+    <t>Lajkovac</t>
+  </si>
+  <si>
+    <t>Lapovo</t>
+  </si>
+  <si>
+    <t>Lebane</t>
+  </si>
+  <si>
+    <t>Leskovac - grad</t>
+  </si>
+  <si>
+    <t>Loznica - grad</t>
+  </si>
+  <si>
+    <t>Lučani</t>
+  </si>
+  <si>
+    <t>Ljig</t>
+  </si>
+  <si>
+    <t>Ljubovija</t>
+  </si>
+  <si>
+    <t>Majdanpek</t>
+  </si>
+  <si>
+    <t>Mali Zvornik</t>
+  </si>
+  <si>
+    <t>Mali Iđoš</t>
+  </si>
+  <si>
+    <t>Malo Crniće</t>
+  </si>
+  <si>
+    <t>Medveđa</t>
+  </si>
+  <si>
+    <t>Merošina</t>
+  </si>
+  <si>
+    <t>Mionica</t>
+  </si>
+  <si>
+    <t>Negotin</t>
+  </si>
+  <si>
+    <t>Niš - grad</t>
+  </si>
+  <si>
+    <t>Nova Varoš</t>
+  </si>
+  <si>
+    <t>Nova Crnja</t>
+  </si>
+  <si>
+    <t>Novi Bečej</t>
+  </si>
+  <si>
+    <t>Novi Kneževac</t>
+  </si>
+  <si>
+    <t>Novi Pazar - grad</t>
+  </si>
+  <si>
+    <t>Novi Sad - grad</t>
+  </si>
+  <si>
+    <t>Opovo</t>
+  </si>
+  <si>
+    <t>Osečina</t>
+  </si>
+  <si>
+    <t>Odžaci</t>
+  </si>
+  <si>
+    <t>Pančevo</t>
+  </si>
+  <si>
+    <t>Paraćin</t>
+  </si>
+  <si>
+    <t>Petrovac na Mlavi</t>
+  </si>
+  <si>
+    <t>Pećinci</t>
+  </si>
+  <si>
+    <t>Pirot - grad</t>
+  </si>
+  <si>
+    <t>Plandište</t>
+  </si>
+  <si>
+    <t>Požarevac - grad</t>
+  </si>
+  <si>
+    <t>Požega</t>
+  </si>
+  <si>
+    <t>Preševo</t>
+  </si>
+  <si>
+    <t>Priboj</t>
+  </si>
+  <si>
+    <t>Prijepolje</t>
+  </si>
+  <si>
+    <t>Prokuplje</t>
+  </si>
+  <si>
+    <t>Ražanj</t>
+  </si>
+  <si>
+    <t>Rača</t>
+  </si>
+  <si>
+    <t>Raška</t>
+  </si>
+  <si>
+    <t>Rekovac</t>
+  </si>
+  <si>
+    <t>Ruma</t>
+  </si>
+  <si>
+    <t>Svilajnac</t>
+  </si>
+  <si>
+    <t>Svrjig</t>
+  </si>
+  <si>
+    <t>Senta</t>
+  </si>
+  <si>
+    <t>Sečanj</t>
+  </si>
+  <si>
+    <t>Sjenica</t>
+  </si>
+  <si>
+    <t>Smederevo - grad</t>
+  </si>
+  <si>
+    <t>Smederevska Palanka</t>
+  </si>
+  <si>
+    <t>Sokobanja</t>
+  </si>
+  <si>
+    <t>Sombor - grad</t>
+  </si>
+  <si>
+    <t>Srbobran</t>
+  </si>
+  <si>
+    <t>Sremska Mitrovica - grad</t>
+  </si>
+  <si>
+    <t>Sremski Karlovci</t>
+  </si>
+  <si>
+    <t>Stara Pazova</t>
+  </si>
+  <si>
+    <t>Subotica - grad</t>
+  </si>
+  <si>
+    <t>Surdulica</t>
+  </si>
+  <si>
+    <t>Temerin</t>
+  </si>
+  <si>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Topola</t>
+  </si>
+  <si>
+    <t>Trgovište</t>
+  </si>
+  <si>
+    <t>Trstenik</t>
+  </si>
+  <si>
+    <t>Tutin</t>
+  </si>
+  <si>
+    <t>Ćićevac</t>
+  </si>
+  <si>
+    <t>Ćuprija</t>
+  </si>
+  <si>
+    <t>Ub</t>
+  </si>
+  <si>
+    <t>Užice - grad</t>
+  </si>
+  <si>
+    <t>Crna Trava</t>
+  </si>
+  <si>
+    <t>Čajetina</t>
+  </si>
+  <si>
+    <t>Čačak - grad</t>
+  </si>
+  <si>
+    <t>Čoka</t>
+  </si>
+  <si>
+    <t>Šabac - grad</t>
+  </si>
+  <si>
+    <t>Šid</t>
+  </si>
+  <si>
+    <t>Užice - Sevojno</t>
+  </si>
+  <si>
+    <t>Užice - Užice</t>
+  </si>
+  <si>
+    <t>Požarevac - Požarevac</t>
+  </si>
+  <si>
+    <t>Požarevac - Kostolac</t>
+  </si>
+  <si>
+    <t>Novi Sad - Petrovaradin</t>
+  </si>
+  <si>
+    <t>Novi Sad - Novi Sad</t>
+  </si>
+  <si>
+    <t>Niš - Medijana</t>
+  </si>
+  <si>
+    <t>Niš - Niška Banja</t>
+  </si>
+  <si>
+    <t>Niš - Palilula</t>
+  </si>
+  <si>
+    <t>Niš - Pantelej</t>
+  </si>
+  <si>
+    <t>Niš - Crveni Krst</t>
+  </si>
+  <si>
+    <t>Vranje - Vranjska Banja</t>
+  </si>
+  <si>
+    <t>Vranje - Vranje</t>
+  </si>
+  <si>
+    <t>Beograd - Čukarica</t>
+  </si>
+  <si>
+    <t>Beograd - Surčin</t>
+  </si>
+  <si>
+    <t>Beograd - Stari Grad</t>
+  </si>
+  <si>
+    <t>Beograd - Sopot</t>
+  </si>
+  <si>
+    <t>Beograd - Savski Venac</t>
+  </si>
+  <si>
+    <t>Beograd - Rakovica</t>
+  </si>
+  <si>
+    <t>Beograd - Palilula</t>
+  </si>
+  <si>
+    <t>Beograd - Obrenovac</t>
+  </si>
+  <si>
+    <t>Beograd - Novi Beograd</t>
+  </si>
+  <si>
+    <t>Beograd - Mladenovac</t>
+  </si>
+  <si>
+    <t>Beograd - Lazarevac</t>
+  </si>
+  <si>
+    <t>Beograd - Zemun</t>
+  </si>
+  <si>
+    <t>Beograd - Zvezdara</t>
+  </si>
+  <si>
+    <t>Beograd - Grocka</t>
+  </si>
+  <si>
+    <t>Beograd - Vračar</t>
+  </si>
+  <si>
+    <t>Beograd - Vozdovac</t>
+  </si>
+  <si>
+    <t>Beograd - Barajevo</t>
   </si>
 </sst>
 </file>
@@ -664,7 +1210,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1157,4 +1703,1702 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
+        <v>delete from Genders; dbcc checkident (Genders, reseed, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,") values(N'",B3,"', N'",C3,"');")</f>
+        <v>insert into Genders(Name, NameLatin) values(N'Male', N'Muški');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,") values(N'",B4,"', N'",C4,"');")</f>
+        <v>insert into Genders(Name, NameLatin) values(N'Female', N'Ženski');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C177"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
+        <v>delete from Municipalities; dbcc checkident (Municipalities, reseed, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
+        <v>insert into Municipalities(Name) values(N'Ada');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" ref="C4:C67" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B4,"');")</f>
+        <v>insert into Municipalities(Name) values(N'Aleksandrovac');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Aleksinac');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Alibunar');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Apatin');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Aranđelovac');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Arilje');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Babušnica');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bajina Bašta');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Batočina');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bač');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bačka Palanka');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bačka Topola');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bački Petrovac');</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bela Palanka');</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bela Crkva');</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - grad');</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Barajevo');</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Vozdovac');</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Vračar');</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Grocka');</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Zvezdara');</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Zemun');</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Lazarevac');</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Mladenovac');</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Novi Beograd');</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Obrenovac');</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Palilula');</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Rakovica');</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Savski Venac');</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Sopot');</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Stari Grad');</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Surčin');</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beograd - Čukarica');</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Beočin');</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bečej');</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Blace');</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bogatić');</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bojnik');</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Boljevac');</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bor');</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bosilegrad');</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Brus');</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Bujanovac');</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Valjevo - grad');</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Varvarin');</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Velika Plana');</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Veliko Gradište');</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vladimirci');</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vladičin Han');</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vlasotince');</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vranje - grad');</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vranje - Vranje');</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vranje - Vranjska Banja');</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vrbas');</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vrnjačka Banja');</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Vršac - grad');</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Gadžin Han');</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Golubac');</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Gornji Milanovac');</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Despotovac');</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Dimitrovgrad');</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Doljevac');</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Žabalj');</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Municipalities(Name) values(N'Žabari');</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="1" t="str">
+        <f t="shared" ref="C68:C131" si="1">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B68,"');")</f>
+        <v>insert into Municipalities(Name) values(N'Žagubica');</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Žitište');</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Žitorađa');</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>125</v>
+      </c>
+      <c r="C71" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Zaječar - grad');</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Zrenjanin - grad');</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Ivanjica');</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Inđija');</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" t="s">
+        <v>129</v>
+      </c>
+      <c r="C75" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Irig');</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" t="s">
+        <v>130</v>
+      </c>
+      <c r="C76" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Jagodina - grad');</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kanjiža');</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kikinda - grad');</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79" t="s">
+        <v>133</v>
+      </c>
+      <c r="C79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kladovo');</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" t="s">
+        <v>134</v>
+      </c>
+      <c r="C80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Knić');</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" t="s">
+        <v>135</v>
+      </c>
+      <c r="C81" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Knjaževac');</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" t="s">
+        <v>136</v>
+      </c>
+      <c r="C82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kovačica');</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kovin');</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kosjerić');</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" t="s">
+        <v>139</v>
+      </c>
+      <c r="C85" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Koceljeva');</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kragujevac - grad');</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" t="s">
+        <v>141</v>
+      </c>
+      <c r="C87" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kraljevo - grad');</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" t="s">
+        <v>142</v>
+      </c>
+      <c r="C88" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Krupanj');</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="B89" t="s">
+        <v>143</v>
+      </c>
+      <c r="C89" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kruševac - grad');</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" t="s">
+        <v>144</v>
+      </c>
+      <c r="C90" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kula');</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="B91" t="s">
+        <v>145</v>
+      </c>
+      <c r="C91" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kuršumlija');</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="B92" t="s">
+        <v>146</v>
+      </c>
+      <c r="C92" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Kučevo');</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93" t="s">
+        <v>147</v>
+      </c>
+      <c r="C93" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Lajkovac');</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94" t="s">
+        <v>148</v>
+      </c>
+      <c r="C94" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Lapovo');</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95" t="s">
+        <v>149</v>
+      </c>
+      <c r="C95" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Lebane');</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="B96" t="s">
+        <v>150</v>
+      </c>
+      <c r="C96" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Leskovac - grad');</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="B97" t="s">
+        <v>151</v>
+      </c>
+      <c r="C97" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Loznica - grad');</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3">
+      <c r="B98" t="s">
+        <v>152</v>
+      </c>
+      <c r="C98" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Lučani');</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" t="s">
+        <v>153</v>
+      </c>
+      <c r="C99" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Ljig');</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3">
+      <c r="B100" t="s">
+        <v>154</v>
+      </c>
+      <c r="C100" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Ljubovija');</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3">
+      <c r="B101" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Majdanpek');</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3">
+      <c r="B102" t="s">
+        <v>156</v>
+      </c>
+      <c r="C102" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Mali Zvornik');</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3">
+      <c r="B103" t="s">
+        <v>157</v>
+      </c>
+      <c r="C103" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Mali Iđoš');</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3">
+      <c r="B104" t="s">
+        <v>158</v>
+      </c>
+      <c r="C104" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Malo Crniće');</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3">
+      <c r="B105" t="s">
+        <v>159</v>
+      </c>
+      <c r="C105" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Medveđa');</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3">
+      <c r="B106" t="s">
+        <v>160</v>
+      </c>
+      <c r="C106" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Merošina');</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3">
+      <c r="B107" t="s">
+        <v>161</v>
+      </c>
+      <c r="C107" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Mionica');</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3">
+      <c r="B108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C108" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Negotin');</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3">
+      <c r="B109" t="s">
+        <v>163</v>
+      </c>
+      <c r="C109" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Niš - grad');</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3">
+      <c r="B110" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C110" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Niš - Medijana');</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3">
+      <c r="B111" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C111" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Niš - Niška Banja');</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3">
+      <c r="B112" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C112" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Niš - Palilula');</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Niš - Pantelej');</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="B114" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C114" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Niš - Crveni Krst');</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="B115" t="s">
+        <v>164</v>
+      </c>
+      <c r="C115" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Nova Varoš');</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3">
+      <c r="B116" t="s">
+        <v>165</v>
+      </c>
+      <c r="C116" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Nova Crnja');</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
+      <c r="B117" t="s">
+        <v>166</v>
+      </c>
+      <c r="C117" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Novi Bečej');</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3">
+      <c r="B118" t="s">
+        <v>167</v>
+      </c>
+      <c r="C118" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Novi Kneževac');</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3">
+      <c r="B119" t="s">
+        <v>168</v>
+      </c>
+      <c r="C119" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Novi Pazar - grad');</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3">
+      <c r="B120" t="s">
+        <v>169</v>
+      </c>
+      <c r="C120" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Novi Sad - grad');</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3">
+      <c r="B121" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Novi Sad - Novi Sad');</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3">
+      <c r="B122" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C122" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Novi Sad - Petrovaradin');</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3">
+      <c r="B123" t="s">
+        <v>170</v>
+      </c>
+      <c r="C123" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Opovo');</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3">
+      <c r="B124" t="s">
+        <v>171</v>
+      </c>
+      <c r="C124" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Osečina');</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3">
+      <c r="B125" t="s">
+        <v>172</v>
+      </c>
+      <c r="C125" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Odžaci');</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3">
+      <c r="B126" t="s">
+        <v>173</v>
+      </c>
+      <c r="C126" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Pančevo');</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3">
+      <c r="B127" t="s">
+        <v>174</v>
+      </c>
+      <c r="C127" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Paraćin');</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3">
+      <c r="B128" t="s">
+        <v>175</v>
+      </c>
+      <c r="C128" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Petrovac na Mlavi');</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3">
+      <c r="B129" t="s">
+        <v>176</v>
+      </c>
+      <c r="C129" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Pećinci');</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3">
+      <c r="B130" t="s">
+        <v>177</v>
+      </c>
+      <c r="C130" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Pirot - grad');</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3">
+      <c r="B131" t="s">
+        <v>178</v>
+      </c>
+      <c r="C131" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Municipalities(Name) values(N'Plandište');</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3">
+      <c r="B132" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" s="1" t="str">
+        <f t="shared" ref="C132:C177" si="2">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B132,"');")</f>
+        <v>insert into Municipalities(Name) values(N'Požarevac - grad');</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3">
+      <c r="B133" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C133" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Požarevac - Kostolac');</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3">
+      <c r="B134" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C134" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Požarevac - Požarevac');</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3">
+      <c r="B135" t="s">
+        <v>180</v>
+      </c>
+      <c r="C135" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Požega');</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3">
+      <c r="B136" t="s">
+        <v>181</v>
+      </c>
+      <c r="C136" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Preševo');</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3">
+      <c r="B137" t="s">
+        <v>182</v>
+      </c>
+      <c r="C137" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Priboj');</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3">
+      <c r="B138" t="s">
+        <v>183</v>
+      </c>
+      <c r="C138" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Prijepolje');</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3">
+      <c r="B139" t="s">
+        <v>184</v>
+      </c>
+      <c r="C139" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Prokuplje');</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3">
+      <c r="B140" t="s">
+        <v>185</v>
+      </c>
+      <c r="C140" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Ražanj');</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3">
+      <c r="B141" t="s">
+        <v>186</v>
+      </c>
+      <c r="C141" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Rača');</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3">
+      <c r="B142" t="s">
+        <v>187</v>
+      </c>
+      <c r="C142" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Raška');</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3">
+      <c r="B143" t="s">
+        <v>188</v>
+      </c>
+      <c r="C143" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Rekovac');</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3">
+      <c r="B144" t="s">
+        <v>189</v>
+      </c>
+      <c r="C144" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Ruma');</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3">
+      <c r="B145" t="s">
+        <v>190</v>
+      </c>
+      <c r="C145" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Svilajnac');</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3">
+      <c r="B146" t="s">
+        <v>191</v>
+      </c>
+      <c r="C146" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Svrjig');</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3">
+      <c r="B147" t="s">
+        <v>192</v>
+      </c>
+      <c r="C147" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Senta');</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3">
+      <c r="B148" t="s">
+        <v>193</v>
+      </c>
+      <c r="C148" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Sečanj');</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3">
+      <c r="B149" t="s">
+        <v>194</v>
+      </c>
+      <c r="C149" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Sjenica');</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3">
+      <c r="B150" t="s">
+        <v>195</v>
+      </c>
+      <c r="C150" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Smederevo - grad');</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3">
+      <c r="B151" t="s">
+        <v>196</v>
+      </c>
+      <c r="C151" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Smederevska Palanka');</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3">
+      <c r="B152" t="s">
+        <v>197</v>
+      </c>
+      <c r="C152" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Sokobanja');</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3">
+      <c r="B153" t="s">
+        <v>198</v>
+      </c>
+      <c r="C153" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Sombor - grad');</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3">
+      <c r="B154" t="s">
+        <v>199</v>
+      </c>
+      <c r="C154" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Srbobran');</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3">
+      <c r="B155" t="s">
+        <v>200</v>
+      </c>
+      <c r="C155" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Sremska Mitrovica - grad');</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3">
+      <c r="B156" t="s">
+        <v>201</v>
+      </c>
+      <c r="C156" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Sremski Karlovci');</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3">
+      <c r="B157" t="s">
+        <v>202</v>
+      </c>
+      <c r="C157" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Stara Pazova');</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3">
+      <c r="B158" t="s">
+        <v>203</v>
+      </c>
+      <c r="C158" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Subotica - grad');</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3">
+      <c r="B159" t="s">
+        <v>204</v>
+      </c>
+      <c r="C159" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Surdulica');</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3">
+      <c r="B160" t="s">
+        <v>205</v>
+      </c>
+      <c r="C160" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Temerin');</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3">
+      <c r="B161" t="s">
+        <v>206</v>
+      </c>
+      <c r="C161" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Titel');</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3">
+      <c r="B162" t="s">
+        <v>207</v>
+      </c>
+      <c r="C162" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Topola');</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3">
+      <c r="B163" t="s">
+        <v>208</v>
+      </c>
+      <c r="C163" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Trgovište');</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3">
+      <c r="B164" t="s">
+        <v>209</v>
+      </c>
+      <c r="C164" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Trstenik');</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3">
+      <c r="B165" t="s">
+        <v>210</v>
+      </c>
+      <c r="C165" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Tutin');</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3">
+      <c r="B166" t="s">
+        <v>211</v>
+      </c>
+      <c r="C166" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Ćićevac');</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3">
+      <c r="B167" t="s">
+        <v>212</v>
+      </c>
+      <c r="C167" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Ćuprija');</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3">
+      <c r="B168" t="s">
+        <v>213</v>
+      </c>
+      <c r="C168" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Ub');</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3">
+      <c r="B169" t="s">
+        <v>214</v>
+      </c>
+      <c r="C169" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Užice - grad');</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3">
+      <c r="B170" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C170" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Užice - Sevojno');</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3">
+      <c r="B171" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C171" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Užice - Užice');</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3">
+      <c r="B172" t="s">
+        <v>215</v>
+      </c>
+      <c r="C172" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Crna Trava');</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3">
+      <c r="B173" t="s">
+        <v>216</v>
+      </c>
+      <c r="C173" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Čajetina');</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3">
+      <c r="B174" t="s">
+        <v>217</v>
+      </c>
+      <c r="C174" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Čačak - grad');</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3">
+      <c r="B175" t="s">
+        <v>218</v>
+      </c>
+      <c r="C175" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Čoka');</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3">
+      <c r="B176" t="s">
+        <v>219</v>
+      </c>
+      <c r="C176" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Šabac - grad');</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3">
+      <c r="B177" t="s">
+        <v>220</v>
+      </c>
+      <c r="C177" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into Municipalities(Name) values(N'Šid');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on the business logic, mainly modeling, apstraction with security package, many to many relationships and inheritance.
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -1209,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1709,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Working on the authorization.
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Genders" sheetId="4" r:id="rId4"/>
     <sheet name="Municipalities" sheetId="5" r:id="rId5"/>
     <sheet name="Companies" sheetId="6" r:id="rId6"/>
+    <sheet name="PartnerPermissions" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="250">
   <si>
     <t>Permissions</t>
   </si>
@@ -30,39 +31,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CreatedAt</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
-    <t>Read roles</t>
-  </si>
-  <si>
-    <t>Edit roles</t>
-  </si>
-  <si>
-    <t>Insert roles</t>
-  </si>
-  <si>
-    <t>Delete roles</t>
-  </si>
-  <si>
-    <t>Read users</t>
-  </si>
-  <si>
-    <t>Edit users</t>
-  </si>
-  <si>
-    <t>Delete users</t>
-  </si>
-  <si>
     <t>NameLatin</t>
   </si>
   <si>
-    <t>DescriptionLatin</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -102,78 +76,12 @@
     <t>Cancelled</t>
   </si>
   <si>
-    <t>Read permissions</t>
-  </si>
-  <si>
-    <t>Read tiers</t>
-  </si>
-  <si>
-    <t>Edit tiers</t>
-  </si>
-  <si>
-    <t>Insert tiers</t>
-  </si>
-  <si>
-    <t>Delete tiers</t>
-  </si>
-  <si>
-    <t>Pregled uloga korisnika</t>
-  </si>
-  <si>
-    <t>Promena uloga korisnika</t>
-  </si>
-  <si>
-    <t>Promena nivoa odanosti</t>
-  </si>
-  <si>
-    <t>Dodavanje uloga korisnika</t>
-  </si>
-  <si>
-    <t>Promena profila korisnika</t>
-  </si>
-  <si>
-    <t>Pregled profila korisnika</t>
-  </si>
-  <si>
-    <t>Brisanje profila korisnika</t>
-  </si>
-  <si>
-    <t>Pregled permisija uloga</t>
-  </si>
-  <si>
     <t>Pregled nivoa odanosti</t>
   </si>
   <si>
-    <t>Dodavanje nivoa odanosti</t>
-  </si>
-  <si>
     <t>Brisanje nivoa odanosti</t>
   </si>
   <si>
-    <t>Brisanje uloga korisnika</t>
-  </si>
-  <si>
-    <t>Read transactions</t>
-  </si>
-  <si>
-    <t>Pregled transakcija</t>
-  </si>
-  <si>
-    <t>Read transaction products</t>
-  </si>
-  <si>
-    <t>Pregled proizvoda iz transakcije</t>
-  </si>
-  <si>
-    <t>Read transaction statuses</t>
-  </si>
-  <si>
-    <t>Pregled statusa transakcije</t>
-  </si>
-  <si>
-    <t>ReadPermission</t>
-  </si>
-  <si>
     <t>InsertTier</t>
   </si>
   <si>
@@ -186,36 +94,9 @@
     <t>DeleteTier</t>
   </si>
   <si>
-    <t>ReadTransaction</t>
-  </si>
-  <si>
-    <t>ReadTransactionProduct</t>
-  </si>
-  <si>
-    <t>ReadTransactionStatus</t>
-  </si>
-  <si>
-    <t>Read notifications</t>
-  </si>
-  <si>
-    <t>Edit notifications</t>
-  </si>
-  <si>
-    <t>Insert notifications</t>
-  </si>
-  <si>
-    <t>Delete notifications</t>
-  </si>
-  <si>
     <t>Pregled notifikacija</t>
   </si>
   <si>
-    <t>Promena notifikacija</t>
-  </si>
-  <si>
-    <t>Dodavanje notifikacija</t>
-  </si>
-  <si>
     <t>Brisanje notifikacija</t>
   </si>
   <si>
@@ -772,6 +653,123 @@
   </si>
   <si>
     <t>Beograd - Barajevo</t>
+  </si>
+  <si>
+    <t>ReadPartner</t>
+  </si>
+  <si>
+    <t>EditPartner</t>
+  </si>
+  <si>
+    <t>InsertPartner</t>
+  </si>
+  <si>
+    <t>DeletePartner</t>
+  </si>
+  <si>
+    <t>Pregled korisnika</t>
+  </si>
+  <si>
+    <t>Brisanje korisnika</t>
+  </si>
+  <si>
+    <t>Dodavanje novih notifikacija</t>
+  </si>
+  <si>
+    <t>Promena postojećih notifikacija</t>
+  </si>
+  <si>
+    <t>Promena postojećih korisnika</t>
+  </si>
+  <si>
+    <t>Pregled partnera</t>
+  </si>
+  <si>
+    <t>Promena postojećih partnera</t>
+  </si>
+  <si>
+    <t>Dodavanje novih partnera</t>
+  </si>
+  <si>
+    <t>Brisanje partnera</t>
+  </si>
+  <si>
+    <t>Pregled uloga</t>
+  </si>
+  <si>
+    <t>Promena postojećih uloga</t>
+  </si>
+  <si>
+    <t>Dodavanje novih uloga</t>
+  </si>
+  <si>
+    <t>Brisanje uloga</t>
+  </si>
+  <si>
+    <t>PartnerPermissions</t>
+  </si>
+  <si>
+    <t>ReadPartnerRole</t>
+  </si>
+  <si>
+    <t>EditPartnerRole</t>
+  </si>
+  <si>
+    <t>InsertPartnerRole</t>
+  </si>
+  <si>
+    <t>DeletePartnerRole</t>
+  </si>
+  <si>
+    <t>ReadPartnerUser</t>
+  </si>
+  <si>
+    <t>EditPartnerUser</t>
+  </si>
+  <si>
+    <t>ReadPartnerNotification</t>
+  </si>
+  <si>
+    <t>EditPartnerNotification</t>
+  </si>
+  <si>
+    <t>InsertPartnerNotification</t>
+  </si>
+  <si>
+    <t>DeletePartnerNotification</t>
+  </si>
+  <si>
+    <t>ReadSegmentation</t>
+  </si>
+  <si>
+    <t>EditSegmentation</t>
+  </si>
+  <si>
+    <t>InsertSegmentation</t>
+  </si>
+  <si>
+    <t>DeleteSegmentation</t>
+  </si>
+  <si>
+    <t>Promena partnera</t>
+  </si>
+  <si>
+    <t>Promena postojećih nivoa odanosti</t>
+  </si>
+  <si>
+    <t>Dodavanje novih nivoa odanosti</t>
+  </si>
+  <si>
+    <t>Pregled segmentacija</t>
+  </si>
+  <si>
+    <t>Promena postojećih segmentacija</t>
+  </si>
+  <si>
+    <t>Dodavanje novih segmentacija</t>
+  </si>
+  <si>
+    <t>Brisanje segmentacija</t>
   </si>
 </sst>
 </file>
@@ -1207,418 +1205,306 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="str">
+      <c r="E2" s="1" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
         <v>delete from Permissions; dbcc checkident (Permissions, reseed, 0);</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="str">
-        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B3,"', N'",C3,"', ",IF(TRIM(D3)&lt;&gt;"","N'"&amp;D3&amp;"'","null"),", ",IF(TRIM(E3)&lt;&gt;"","N'"&amp;E3&amp;"'","null")," , getdate(), N'",G3,"');")</f>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read roles', N'Pregled uloga korisnika', null, null , getdate(), N'ReadRole');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="B3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', ",IF(TRIM(C3)&lt;&gt;"","N'"&amp;C3&amp;"'","null"),", N'",D3,"');")</f>
+        <v>insert into Permissions(Name, Description, Code) values(N'Pregled korisnika', null, N'ReadUserExtended');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f t="shared" ref="H4:H21" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values(N'",B4,"', N'",C4,"', ",IF(TRIM(D4)&lt;&gt;"","N'"&amp;D4&amp;"'","null"),", ",IF(TRIM(E4)&lt;&gt;"","N'"&amp;E4&amp;"'","null")," , getdate(), N'",G4,"');")</f>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit roles', N'Promena uloga korisnika', null, null , getdate(), N'EditRole');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="B4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4:E17" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
+        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih korisnika', null, N'EditUserExtended');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert roles', N'Dodavanje uloga korisnika', null, null , getdate(), N'InsertRole');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="B5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje korisnika', null, N'DeleteUserExtended');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete roles', N'Brisanje uloga korisnika', null, null , getdate(), N'DeleteRole');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Pregled notifikacija', null, N'ReadNotification');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read users', N'Pregled profila korisnika', null, null , getdate(), N'ReadUserExtended');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="B7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih notifikacija', null, N'EditNotification');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit users', N'Promena profila korisnika', null, null , getdate(), N'EditUserExtended');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="B8" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Dodavanje novih notifikacija', null, N'InsertNotification');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete users', N'Brisanje profila korisnika', null, null , getdate(), N'DeleteUserExtended');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje notifikacija', null, N'DeleteNotification');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read permissions', N'Pregled permisija uloga', null, null , getdate(), N'ReadPermission');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>220</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read tiers', N'Pregled nivoa odanosti', null, null , getdate(), N'ReadTier');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>221</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih partnera', null, N'EditPartner');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit tiers', N'Promena nivoa odanosti', null, null , getdate(), N'EditTier');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>222</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Dodavanje novih partnera', null, N'InsertPartner');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert tiers', N'Dodavanje nivoa odanosti', null, null , getdate(), N'InsertTier');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>223</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje partnera', null, N'DeletePartner');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete tiers', N'Brisanje nivoa odanosti', null, null , getdate(), N'DeleteTier');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>224</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Pregled uloga', null, N'ReadRole');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transactions', N'Pregled transakcija', null, null , getdate(), N'ReadTransaction');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>225</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih uloga', null, N'EditRole');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transaction products', N'Pregled proizvoda iz transakcije', null, null , getdate(), N'ReadTransactionProduct');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>226</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Dodavanje novih uloga', null, N'InsertRole');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read transaction statuses', N'Pregled statusa transakcije', null, null , getdate(), N'ReadTransactionStatus');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje uloga', null, N'DeleteRole');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Read notifications', N'Pregled notifikacija', null, null , getdate(), N'ReadNotification');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>63</v>
-      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Edit notifications', N'Promena notifikacija', null, null , getdate(), N'EditNotification');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Insert notifications', N'Dodavanje notifikacija', null, null , getdate(), N'InsertNotification');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, NameLatin, Description, DescriptionLatin, CreatedAt, Code) values(N'Delete notifications', N'Brisanje notifikacija', null, null , getdate(), N'DeleteNotification');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1643,21 +1529,21 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
@@ -1669,13 +1555,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', N'",C3,"', N'",D3,"');")</f>
@@ -1687,13 +1573,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', N'",C4,"', N'",D4,"');")</f>
@@ -1709,7 +1595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1722,20 +1608,20 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
@@ -1747,10 +1633,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,") values(N'",B3,"', N'",C3,"');")</f>
@@ -1762,10 +1648,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,") values(N'",B4,"', N'",C4,"');")</f>
@@ -1782,7 +1668,7 @@
   <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1794,12 +1680,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1811,7 +1697,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
@@ -1820,7 +1706,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C67" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B4,"');")</f>
@@ -1829,7 +1715,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1838,7 +1724,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1847,7 +1733,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1856,7 +1742,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1865,7 +1751,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1874,7 +1760,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1883,7 +1769,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1892,7 +1778,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1901,7 +1787,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1910,7 +1796,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1919,7 +1805,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1928,7 +1814,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1937,7 +1823,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1946,7 +1832,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1955,7 +1841,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1964,7 +1850,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="1" t="s">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1973,7 +1859,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="1" t="s">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1982,7 +1868,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="1" t="s">
-        <v>248</v>
+        <v>208</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1991,7 +1877,7 @@
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="1" t="s">
-        <v>247</v>
+        <v>207</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2000,7 +1886,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="1" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2009,7 +1895,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="1" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2018,7 +1904,7 @@
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="1" t="s">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2027,7 +1913,7 @@
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="1" t="s">
-        <v>243</v>
+        <v>203</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2036,7 +1922,7 @@
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="1" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="C28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2045,7 +1931,7 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="1" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="C29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2054,7 +1940,7 @@
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="1" t="s">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="C30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2063,7 +1949,7 @@
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="1" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2072,7 +1958,7 @@
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="1" t="s">
-        <v>238</v>
+        <v>198</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2081,7 +1967,7 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="1" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2090,7 +1976,7 @@
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="1" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2099,7 +1985,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="1" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="C35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2108,7 +1994,7 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="1" t="s">
-        <v>234</v>
+        <v>194</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2117,7 +2003,7 @@
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2126,7 +2012,7 @@
     </row>
     <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2135,7 +2021,7 @@
     </row>
     <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2144,7 +2030,7 @@
     </row>
     <row r="40" spans="2:3">
       <c r="B40" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2153,7 +2039,7 @@
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2162,7 +2048,7 @@
     </row>
     <row r="42" spans="2:3">
       <c r="B42" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2171,7 +2057,7 @@
     </row>
     <row r="43" spans="2:3">
       <c r="B43" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2180,7 +2066,7 @@
     </row>
     <row r="44" spans="2:3">
       <c r="B44" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2189,7 +2075,7 @@
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2198,7 +2084,7 @@
     </row>
     <row r="46" spans="2:3">
       <c r="B46" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2207,7 +2093,7 @@
     </row>
     <row r="47" spans="2:3">
       <c r="B47" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2216,7 +2102,7 @@
     </row>
     <row r="48" spans="2:3">
       <c r="B48" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2225,7 +2111,7 @@
     </row>
     <row r="49" spans="2:3">
       <c r="B49" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="C49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2234,7 +2120,7 @@
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2243,7 +2129,7 @@
     </row>
     <row r="51" spans="2:3">
       <c r="B51" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2252,7 +2138,7 @@
     </row>
     <row r="52" spans="2:3">
       <c r="B52" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="C52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2261,7 +2147,7 @@
     </row>
     <row r="53" spans="2:3">
       <c r="B53" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="C53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2270,7 +2156,7 @@
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="C54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2279,7 +2165,7 @@
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="1" t="s">
-        <v>233</v>
+        <v>193</v>
       </c>
       <c r="C55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2288,7 +2174,7 @@
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="1" t="s">
-        <v>232</v>
+        <v>192</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2297,7 +2183,7 @@
     </row>
     <row r="57" spans="2:3">
       <c r="B57" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2306,7 +2192,7 @@
     </row>
     <row r="58" spans="2:3">
       <c r="B58" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2315,7 +2201,7 @@
     </row>
     <row r="59" spans="2:3">
       <c r="B59" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2324,7 +2210,7 @@
     </row>
     <row r="60" spans="2:3">
       <c r="B60" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="C60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2333,7 +2219,7 @@
     </row>
     <row r="61" spans="2:3">
       <c r="B61" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2342,7 +2228,7 @@
     </row>
     <row r="62" spans="2:3">
       <c r="B62" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2351,7 +2237,7 @@
     </row>
     <row r="63" spans="2:3">
       <c r="B63" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2360,7 +2246,7 @@
     </row>
     <row r="64" spans="2:3">
       <c r="B64" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="C64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2369,7 +2255,7 @@
     </row>
     <row r="65" spans="2:3">
       <c r="B65" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="C65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2378,7 +2264,7 @@
     </row>
     <row r="66" spans="2:3">
       <c r="B66" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="C66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2387,7 +2273,7 @@
     </row>
     <row r="67" spans="2:3">
       <c r="B67" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="C67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2396,7 +2282,7 @@
     </row>
     <row r="68" spans="2:3">
       <c r="B68" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="C68" s="1" t="str">
         <f t="shared" ref="C68:C131" si="1">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B68,"');")</f>
@@ -2405,7 +2291,7 @@
     </row>
     <row r="69" spans="2:3">
       <c r="B69" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2414,7 +2300,7 @@
     </row>
     <row r="70" spans="2:3">
       <c r="B70" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="C70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2423,7 +2309,7 @@
     </row>
     <row r="71" spans="2:3">
       <c r="B71" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="C71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2432,7 +2318,7 @@
     </row>
     <row r="72" spans="2:3">
       <c r="B72" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="C72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2441,7 +2327,7 @@
     </row>
     <row r="73" spans="2:3">
       <c r="B73" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="C73" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2450,7 +2336,7 @@
     </row>
     <row r="74" spans="2:3">
       <c r="B74" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C74" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2459,7 +2345,7 @@
     </row>
     <row r="75" spans="2:3">
       <c r="B75" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2468,7 +2354,7 @@
     </row>
     <row r="76" spans="2:3">
       <c r="B76" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="C76" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2477,7 +2363,7 @@
     </row>
     <row r="77" spans="2:3">
       <c r="B77" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="C77" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2486,7 +2372,7 @@
     </row>
     <row r="78" spans="2:3">
       <c r="B78" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="C78" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2495,7 +2381,7 @@
     </row>
     <row r="79" spans="2:3">
       <c r="B79" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="C79" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2504,7 +2390,7 @@
     </row>
     <row r="80" spans="2:3">
       <c r="B80" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="C80" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2513,7 +2399,7 @@
     </row>
     <row r="81" spans="2:3">
       <c r="B81" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="C81" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2522,7 +2408,7 @@
     </row>
     <row r="82" spans="2:3">
       <c r="B82" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2531,7 +2417,7 @@
     </row>
     <row r="83" spans="2:3">
       <c r="B83" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="C83" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2540,7 +2426,7 @@
     </row>
     <row r="84" spans="2:3">
       <c r="B84" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="C84" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2549,7 +2435,7 @@
     </row>
     <row r="85" spans="2:3">
       <c r="B85" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="C85" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2558,7 +2444,7 @@
     </row>
     <row r="86" spans="2:3">
       <c r="B86" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="C86" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2567,7 +2453,7 @@
     </row>
     <row r="87" spans="2:3">
       <c r="B87" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="C87" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2576,7 +2462,7 @@
     </row>
     <row r="88" spans="2:3">
       <c r="B88" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="C88" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2585,7 +2471,7 @@
     </row>
     <row r="89" spans="2:3">
       <c r="B89" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
       <c r="C89" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2594,7 +2480,7 @@
     </row>
     <row r="90" spans="2:3">
       <c r="B90" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="C90" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2603,7 +2489,7 @@
     </row>
     <row r="91" spans="2:3">
       <c r="B91" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="C91" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2612,7 +2498,7 @@
     </row>
     <row r="92" spans="2:3">
       <c r="B92" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C92" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2621,7 +2507,7 @@
     </row>
     <row r="93" spans="2:3">
       <c r="B93" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="C93" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2630,7 +2516,7 @@
     </row>
     <row r="94" spans="2:3">
       <c r="B94" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="C94" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2639,7 +2525,7 @@
     </row>
     <row r="95" spans="2:3">
       <c r="B95" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="C95" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2648,7 +2534,7 @@
     </row>
     <row r="96" spans="2:3">
       <c r="B96" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="C96" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2657,7 +2543,7 @@
     </row>
     <row r="97" spans="2:3">
       <c r="B97" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="C97" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2666,7 +2552,7 @@
     </row>
     <row r="98" spans="2:3">
       <c r="B98" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="C98" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2675,7 +2561,7 @@
     </row>
     <row r="99" spans="2:3">
       <c r="B99" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="C99" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2684,7 +2570,7 @@
     </row>
     <row r="100" spans="2:3">
       <c r="B100" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="C100" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2693,7 +2579,7 @@
     </row>
     <row r="101" spans="2:3">
       <c r="B101" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="C101" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2702,7 +2588,7 @@
     </row>
     <row r="102" spans="2:3">
       <c r="B102" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="C102" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2711,7 +2597,7 @@
     </row>
     <row r="103" spans="2:3">
       <c r="B103" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="C103" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2720,7 +2606,7 @@
     </row>
     <row r="104" spans="2:3">
       <c r="B104" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="C104" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2729,7 +2615,7 @@
     </row>
     <row r="105" spans="2:3">
       <c r="B105" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
       <c r="C105" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2738,7 +2624,7 @@
     </row>
     <row r="106" spans="2:3">
       <c r="B106" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="C106" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2747,7 +2633,7 @@
     </row>
     <row r="107" spans="2:3">
       <c r="B107" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C107" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2756,7 +2642,7 @@
     </row>
     <row r="108" spans="2:3">
       <c r="B108" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="C108" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2765,7 +2651,7 @@
     </row>
     <row r="109" spans="2:3">
       <c r="B109" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="C109" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2774,7 +2660,7 @@
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="1" t="s">
-        <v>227</v>
+        <v>187</v>
       </c>
       <c r="C110" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2783,7 +2669,7 @@
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="1" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="C111" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2792,7 +2678,7 @@
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="1" t="s">
-        <v>229</v>
+        <v>189</v>
       </c>
       <c r="C112" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2801,7 +2687,7 @@
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="1" t="s">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="C113" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2810,7 +2696,7 @@
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="1" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="C114" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2819,7 +2705,7 @@
     </row>
     <row r="115" spans="2:3">
       <c r="B115" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="C115" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2828,7 +2714,7 @@
     </row>
     <row r="116" spans="2:3">
       <c r="B116" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="C116" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2837,7 +2723,7 @@
     </row>
     <row r="117" spans="2:3">
       <c r="B117" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="C117" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2846,7 +2732,7 @@
     </row>
     <row r="118" spans="2:3">
       <c r="B118" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="C118" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2855,7 +2741,7 @@
     </row>
     <row r="119" spans="2:3">
       <c r="B119" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="C119" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2864,7 +2750,7 @@
     </row>
     <row r="120" spans="2:3">
       <c r="B120" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="C120" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2873,7 +2759,7 @@
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="1" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="C121" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2882,7 +2768,7 @@
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="1" t="s">
-        <v>225</v>
+        <v>185</v>
       </c>
       <c r="C122" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2891,7 +2777,7 @@
     </row>
     <row r="123" spans="2:3">
       <c r="B123" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="C123" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2900,7 +2786,7 @@
     </row>
     <row r="124" spans="2:3">
       <c r="B124" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="C124" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2909,7 +2795,7 @@
     </row>
     <row r="125" spans="2:3">
       <c r="B125" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="C125" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2918,7 +2804,7 @@
     </row>
     <row r="126" spans="2:3">
       <c r="B126" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="C126" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2927,7 +2813,7 @@
     </row>
     <row r="127" spans="2:3">
       <c r="B127" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="C127" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2936,7 +2822,7 @@
     </row>
     <row r="128" spans="2:3">
       <c r="B128" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="C128" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2945,7 +2831,7 @@
     </row>
     <row r="129" spans="2:3">
       <c r="B129" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="C129" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2954,7 +2840,7 @@
     </row>
     <row r="130" spans="2:3">
       <c r="B130" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="C130" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2963,7 +2849,7 @@
     </row>
     <row r="131" spans="2:3">
       <c r="B131" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="C131" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2972,7 +2858,7 @@
     </row>
     <row r="132" spans="2:3">
       <c r="B132" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="C132" s="1" t="str">
         <f t="shared" ref="C132:C177" si="2">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B132,"');")</f>
@@ -2981,7 +2867,7 @@
     </row>
     <row r="133" spans="2:3">
       <c r="B133" s="1" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="C133" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2990,7 +2876,7 @@
     </row>
     <row r="134" spans="2:3">
       <c r="B134" s="1" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="C134" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2999,7 +2885,7 @@
     </row>
     <row r="135" spans="2:3">
       <c r="B135" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C135" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3008,7 +2894,7 @@
     </row>
     <row r="136" spans="2:3">
       <c r="B136" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="C136" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3017,7 +2903,7 @@
     </row>
     <row r="137" spans="2:3">
       <c r="B137" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="C137" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3026,7 +2912,7 @@
     </row>
     <row r="138" spans="2:3">
       <c r="B138" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="C138" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3035,7 +2921,7 @@
     </row>
     <row r="139" spans="2:3">
       <c r="B139" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="C139" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3044,7 +2930,7 @@
     </row>
     <row r="140" spans="2:3">
       <c r="B140" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="C140" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3053,7 +2939,7 @@
     </row>
     <row r="141" spans="2:3">
       <c r="B141" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="C141" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3062,7 +2948,7 @@
     </row>
     <row r="142" spans="2:3">
       <c r="B142" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="C142" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3071,7 +2957,7 @@
     </row>
     <row r="143" spans="2:3">
       <c r="B143" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="C143" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3080,7 +2966,7 @@
     </row>
     <row r="144" spans="2:3">
       <c r="B144" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="C144" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3089,7 +2975,7 @@
     </row>
     <row r="145" spans="2:3">
       <c r="B145" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="C145" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3098,7 +2984,7 @@
     </row>
     <row r="146" spans="2:3">
       <c r="B146" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="C146" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3107,7 +2993,7 @@
     </row>
     <row r="147" spans="2:3">
       <c r="B147" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="C147" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3116,7 +3002,7 @@
     </row>
     <row r="148" spans="2:3">
       <c r="B148" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="C148" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3125,7 +3011,7 @@
     </row>
     <row r="149" spans="2:3">
       <c r="B149" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="C149" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3134,7 +3020,7 @@
     </row>
     <row r="150" spans="2:3">
       <c r="B150" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="C150" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3143,7 +3029,7 @@
     </row>
     <row r="151" spans="2:3">
       <c r="B151" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="C151" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3152,7 +3038,7 @@
     </row>
     <row r="152" spans="2:3">
       <c r="B152" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="C152" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3161,7 +3047,7 @@
     </row>
     <row r="153" spans="2:3">
       <c r="B153" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="C153" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3170,7 +3056,7 @@
     </row>
     <row r="154" spans="2:3">
       <c r="B154" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="C154" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3179,7 +3065,7 @@
     </row>
     <row r="155" spans="2:3">
       <c r="B155" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="C155" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3188,7 +3074,7 @@
     </row>
     <row r="156" spans="2:3">
       <c r="B156" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="C156" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3197,7 +3083,7 @@
     </row>
     <row r="157" spans="2:3">
       <c r="B157" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="C157" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3206,7 +3092,7 @@
     </row>
     <row r="158" spans="2:3">
       <c r="B158" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="C158" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3215,7 +3101,7 @@
     </row>
     <row r="159" spans="2:3">
       <c r="B159" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="C159" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3224,7 +3110,7 @@
     </row>
     <row r="160" spans="2:3">
       <c r="B160" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="C160" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3233,7 +3119,7 @@
     </row>
     <row r="161" spans="2:3">
       <c r="B161" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="C161" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3242,7 +3128,7 @@
     </row>
     <row r="162" spans="2:3">
       <c r="B162" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="C162" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3251,7 +3137,7 @@
     </row>
     <row r="163" spans="2:3">
       <c r="B163" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="C163" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3260,7 +3146,7 @@
     </row>
     <row r="164" spans="2:3">
       <c r="B164" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
       <c r="C164" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3269,7 +3155,7 @@
     </row>
     <row r="165" spans="2:3">
       <c r="B165" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="C165" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3278,7 +3164,7 @@
     </row>
     <row r="166" spans="2:3">
       <c r="B166" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="C166" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3287,7 +3173,7 @@
     </row>
     <row r="167" spans="2:3">
       <c r="B167" t="s">
-        <v>212</v>
+        <v>172</v>
       </c>
       <c r="C167" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3296,7 +3182,7 @@
     </row>
     <row r="168" spans="2:3">
       <c r="B168" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="C168" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3305,7 +3191,7 @@
     </row>
     <row r="169" spans="2:3">
       <c r="B169" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="C169" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3314,7 +3200,7 @@
     </row>
     <row r="170" spans="2:3">
       <c r="B170" s="1" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
       <c r="C170" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3323,7 +3209,7 @@
     </row>
     <row r="171" spans="2:3">
       <c r="B171" s="1" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="C171" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3332,7 +3218,7 @@
     </row>
     <row r="172" spans="2:3">
       <c r="B172" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="C172" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3341,7 +3227,7 @@
     </row>
     <row r="173" spans="2:3">
       <c r="B173" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="C173" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3350,7 +3236,7 @@
     </row>
     <row r="174" spans="2:3">
       <c r="B174" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="C174" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3359,7 +3245,7 @@
     </row>
     <row r="175" spans="2:3">
       <c r="B175" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="C175" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3368,7 +3254,7 @@
     </row>
     <row r="176" spans="2:3">
       <c r="B176" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="C176" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3377,7 +3263,7 @@
     </row>
     <row r="177" spans="2:3">
       <c r="B177" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C177" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3401,4 +3287,429 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
+        <v>delete from PartnerPermissions; dbcc checkident (PartnerPermissions, reseed, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', ",IF(TRIM(C3)&lt;&gt;"","N'"&amp;C3&amp;"'","null"),", N'",D3,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled uloga', null, N'ReadPartnerRole');</v>
+      </c>
+      <c r="R3" t="str">
+        <f>CONCATENATE(D3, " = ", A3, ",")</f>
+        <v>ReadPartnerRole = 1,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4:E22" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih uloga', null, N'EditPartnerRole');</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f t="shared" ref="R4:R22" si="1">CONCATENATE(D4, " = ", A4, ",")</f>
+        <v>EditPartnerRole = 2,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih uloga', null, N'InsertPartnerRole');</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>InsertPartnerRole = 3,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje uloga', null, N'DeletePartnerRole');</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DeletePartnerRole = 4,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled korisnika', null, N'ReadPartnerUser');</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ReadPartnerUser = 5,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih korisnika', null, N'EditPartnerUser');</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EditPartnerUser = 6,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled notifikacija', null, N'ReadPartnerNotification');</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ReadPartnerNotification = 7,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih notifikacija', null, N'EditPartnerNotification');</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EditPartnerNotification = 8,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih notifikacija', null, N'InsertPartnerNotification');</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>InsertPartnerNotification = 9,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje notifikacija', null, N'DeletePartnerNotification');</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DeletePartnerNotification = 10,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ReadPartner = 11,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena partnera', null, N'EditPartner');</v>
+      </c>
+      <c r="R14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EditPartner = 12,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled nivoa odanosti', null, N'ReadTier');</v>
+      </c>
+      <c r="R15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ReadTier = 13,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih nivoa odanosti', null, N'EditTier');</v>
+      </c>
+      <c r="R16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EditTier = 14,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih nivoa odanosti', null, N'InsertTier');</v>
+      </c>
+      <c r="R17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>InsertTier = 15,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje nivoa odanosti', null, N'DeleteTier');</v>
+      </c>
+      <c r="R18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DeleteTier = 16,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled segmentacija', null, N'ReadSegmentation');</v>
+      </c>
+      <c r="R19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>ReadSegmentation = 17,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih segmentacija', null, N'EditSegmentation');</v>
+      </c>
+      <c r="R20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EditSegmentation = 18,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih segmentacija', null, N'InsertSegmentation');</v>
+      </c>
+      <c r="R21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>InsertSegmentation = 19,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje segmentacija', null, N'DeleteSegmentation');</v>
+      </c>
+      <c r="R22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DeleteSegmentation = 20,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the slug in locale storage when saving partner; Added webp to the file upload; Removed points for the gender and birth day; Deleted partner guard, users now make their profiles;
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="251">
   <si>
     <t>Permissions</t>
   </si>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>Brisanje segmentacija</t>
+  </si>
+  <si>
+    <t>DeletePartnerUser</t>
   </si>
 </sst>
 </file>
@@ -3291,10 +3294,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3359,11 +3362,11 @@
         <v>230</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f t="shared" ref="E4:E22" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
+        <f t="shared" ref="E4:E9" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
         <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih uloga', null, N'EditPartnerRole');</v>
       </c>
       <c r="R4" s="1" t="str">
-        <f t="shared" ref="R4:R22" si="1">CONCATENATE(D4, " = ", A4, ",")</f>
+        <f t="shared" ref="R4:R9" si="1">CONCATENATE(D4, " = ", A4, ",")</f>
         <v>EditPartnerRole = 2,</v>
       </c>
     </row>
@@ -3448,18 +3451,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>216</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled notifikacija', null, N'ReadPartnerNotification');</v>
-      </c>
-      <c r="R9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>ReadPartnerNotification = 7,</v>
+        <v>250</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje korisnika', null, N'DeletePartnerUser');</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="1"/>
+        <v>DeletePartnerUser = 7,</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -3467,18 +3470,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih notifikacija', null, N'EditPartnerNotification');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B10,"', ",IF(TRIM(C10)&lt;&gt;"","N'"&amp;C10&amp;"'","null"),", N'",D10,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled notifikacija', null, N'ReadPartnerNotification');</v>
       </c>
       <c r="R10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>EditPartnerNotification = 8,</v>
+        <f>CONCATENATE(D10, " = ", A10, ",")</f>
+        <v>ReadPartnerNotification = 8,</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -3486,18 +3489,18 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih notifikacija', null, N'InsertPartnerNotification');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B11,"', ",IF(TRIM(C11)&lt;&gt;"","N'"&amp;C11&amp;"'","null"),", N'",D11,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih notifikacija', null, N'EditPartnerNotification');</v>
       </c>
       <c r="R11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>InsertPartnerNotification = 9,</v>
+        <f>CONCATENATE(D11, " = ", A11, ",")</f>
+        <v>EditPartnerNotification = 9,</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -3505,18 +3508,18 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje notifikacija', null, N'DeletePartnerNotification');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B12,"', ",IF(TRIM(C12)&lt;&gt;"","N'"&amp;C12&amp;"'","null"),", N'",D12,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih notifikacija', null, N'InsertPartnerNotification');</v>
       </c>
       <c r="R12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>DeletePartnerNotification = 10,</v>
+        <f>CONCATENATE(D12, " = ", A12, ",")</f>
+        <v>InsertPartnerNotification = 10,</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -3524,18 +3527,18 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B13,"', ",IF(TRIM(C13)&lt;&gt;"","N'"&amp;C13&amp;"'","null"),", N'",D13,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje notifikacija', null, N'DeletePartnerNotification');</v>
       </c>
       <c r="R13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>ReadPartner = 11,</v>
+        <f>CONCATENATE(D13, " = ", A13, ",")</f>
+        <v>DeletePartnerNotification = 11,</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -3543,18 +3546,18 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena partnera', null, N'EditPartner');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B14,"', ",IF(TRIM(C14)&lt;&gt;"","N'"&amp;C14&amp;"'","null"),", N'",D14,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
       </c>
       <c r="R14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>EditPartner = 12,</v>
+        <f>CONCATENATE(D14, " = ", A14, ",")</f>
+        <v>ReadPartner = 12,</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -3562,18 +3565,18 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>243</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled nivoa odanosti', null, N'ReadTier');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B15,"', ",IF(TRIM(C15)&lt;&gt;"","N'"&amp;C15&amp;"'","null"),", N'",D15,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena partnera', null, N'EditPartner');</v>
       </c>
       <c r="R15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>ReadTier = 13,</v>
+        <f>CONCATENATE(D15, " = ", A15, ",")</f>
+        <v>EditPartner = 13,</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -3581,18 +3584,18 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih nivoa odanosti', null, N'EditTier');</v>
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B16,"', ",IF(TRIM(C16)&lt;&gt;"","N'"&amp;C16&amp;"'","null"),", N'",D16,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled nivoa odanosti', null, N'ReadTier');</v>
       </c>
       <c r="R16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>EditTier = 14,</v>
+        <f>CONCATENATE(D16, " = ", A16, ",")</f>
+        <v>ReadTier = 14,</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -3600,18 +3603,18 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih nivoa odanosti', null, N'InsertTier');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B17,"', ",IF(TRIM(C17)&lt;&gt;"","N'"&amp;C17&amp;"'","null"),", N'",D17,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih nivoa odanosti', null, N'EditTier');</v>
       </c>
       <c r="R17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>InsertTier = 15,</v>
+        <f>CONCATENATE(D17, " = ", A17, ",")</f>
+        <v>EditTier = 15,</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -3619,18 +3622,18 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje nivoa odanosti', null, N'DeleteTier');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B18,"', ",IF(TRIM(C18)&lt;&gt;"","N'"&amp;C18&amp;"'","null"),", N'",D18,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih nivoa odanosti', null, N'InsertTier');</v>
       </c>
       <c r="R18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>DeleteTier = 16,</v>
+        <f>CONCATENATE(D18, " = ", A18, ",")</f>
+        <v>InsertTier = 16,</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -3638,18 +3641,18 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>239</v>
+        <v>23</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled segmentacija', null, N'ReadSegmentation');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B19,"', ",IF(TRIM(C19)&lt;&gt;"","N'"&amp;C19&amp;"'","null"),", N'",D19,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje nivoa odanosti', null, N'DeleteTier');</v>
       </c>
       <c r="R19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>ReadSegmentation = 17,</v>
+        <f>CONCATENATE(D19, " = ", A19, ",")</f>
+        <v>DeleteTier = 17,</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -3657,18 +3660,18 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih segmentacija', null, N'EditSegmentation');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B20,"', ",IF(TRIM(C20)&lt;&gt;"","N'"&amp;C20&amp;"'","null"),", N'",D20,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Pregled segmentacija', null, N'ReadSegmentation');</v>
       </c>
       <c r="R20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>EditSegmentation = 18,</v>
+        <f>CONCATENATE(D20, " = ", A20, ",")</f>
+        <v>ReadSegmentation = 18,</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -3676,18 +3679,18 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih segmentacija', null, N'InsertSegmentation');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B21,"', ",IF(TRIM(C21)&lt;&gt;"","N'"&amp;C21&amp;"'","null"),", N'",D21,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Promena postojećih segmentacija', null, N'EditSegmentation');</v>
       </c>
       <c r="R21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>InsertSegmentation = 19,</v>
+        <f>CONCATENATE(D21, " = ", A21, ",")</f>
+        <v>EditSegmentation = 19,</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -3695,18 +3698,37 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E22" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B22,"', ",IF(TRIM(C22)&lt;&gt;"","N'"&amp;C22&amp;"'","null"),", N'",D22,"');")</f>
+        <v>insert into PartnerPermissions(Name, Description, Code) values(N'Dodavanje novih segmentacija', null, N'InsertSegmentation');</v>
+      </c>
+      <c r="R22" s="1" t="str">
+        <f>CONCATENATE(D22, " = ", A22, ",")</f>
+        <v>InsertSegmentation = 20,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E22" t="str">
-        <f t="shared" si="0"/>
+      <c r="E23" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B23,"', ",IF(TRIM(C23)&lt;&gt;"","N'"&amp;C23&amp;"'","null"),", N'",D23,"');")</f>
         <v>insert into PartnerPermissions(Name, Description, Code) values(N'Brisanje segmentacija', null, N'DeleteSegmentation');</v>
       </c>
-      <c r="R22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>DeleteSegmentation = 20,</v>
+      <c r="R23" s="1" t="str">
+        <f>CONCATENATE(D23, " = ", A23, ",")</f>
+        <v>DeleteSegmentation = 21,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished showing the data to the user based on his permissions on the Tier page; Fixed issue with not authorized accessing partners data;
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="261">
   <si>
     <t>Permissions</t>
   </si>
@@ -797,6 +797,12 @@
   </si>
   <si>
     <t>UpdateRole</t>
+  </si>
+  <si>
+    <t>ReadCurrentPartner</t>
+  </si>
+  <si>
+    <t>UpdateCurrentPartner</t>
   </si>
 </sst>
 </file>
@@ -1234,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3320,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3573,15 +3579,15 @@
         <v>213</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>205</v>
+        <v>259</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>insert into PartnerPermission(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
+        <v>insert into PartnerPermission(Name, Description, Code) values(N'Pregled partnera', null, N'ReadCurrentPartner');</v>
       </c>
       <c r="R14" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ReadPartner = 12,</v>
+        <v>ReadCurrentPartner = 12,</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -3592,15 +3598,15 @@
         <v>231</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>insert into PartnerPermission(Name, Description, Code) values(N'Promena partnera', null, N'UpdatePartner');</v>
+        <v>insert into PartnerPermission(Name, Description, Code) values(N'Promena partnera', null, N'UpdateCurrentPartner');</v>
       </c>
       <c r="R15" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>UpdatePartner = 13,</v>
+        <v>UpdateCurrentPartner = 13,</v>
       </c>
     </row>
     <row r="16" spans="1:18">

</xml_diff>

<commit_message>
Showing partner-select page always; Showing profile page always; Improved dashboard no partner message;
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="261">
-  <si>
-    <t>Permissions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="259">
   <si>
     <t>Name</t>
   </si>
@@ -94,21 +91,12 @@
     <t>DeleteNotification</t>
   </si>
   <si>
-    <t>Genders</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>Muški</t>
-  </si>
-  <si>
-    <t>Ženski</t>
-  </si>
-  <si>
     <t>Municipalities</t>
   </si>
   <si>
@@ -803,6 +791,12 @@
   </si>
   <si>
     <t>UpdateCurrentPartner</t>
+  </si>
+  <si>
+    <t>Permission</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1235,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E3" sqref="E3:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1253,26 +1247,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
       <c r="E2" s="1" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
-        <v>delete from Permissions; dbcc checkident (Permissions, reseed, 0);</v>
+        <v>delete from Permission; dbcc checkident (Permission, reseed, 0);</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1280,14 +1274,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', ",IF(TRIM(C3)&lt;&gt;"","N'"&amp;C3&amp;"'","null"),", N'",D3,"');")</f>
-        <v>insert into Permissions(Name, Description, Code) values(N'Pregled korisnika', null, N'ReadUserExtended');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Pregled korisnika', null, N'ReadUserExtended');</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1295,14 +1289,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" ref="E4:E17" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
-        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih korisnika', null, N'UpdateUserExtended');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Promena postojećih korisnika', null, N'UpdateUserExtended');</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1310,14 +1304,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje korisnika', null, N'DeleteUserExtended');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Brisanje korisnika', null, N'DeleteUserExtended');</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1325,14 +1319,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Pregled notifikacija', null, N'ReadNotification');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Pregled notifikacija', null, N'ReadNotification');</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1340,14 +1334,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih notifikacija', null, N'UpdateNotification');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Promena postojećih notifikacija', null, N'UpdateNotification');</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1355,14 +1349,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Dodavanje novih notifikacija', null, N'InsertNotification');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Dodavanje novih notifikacija', null, N'InsertNotification');</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1370,14 +1364,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje notifikacija', null, N'DeleteNotification');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Brisanje notifikacija', null, N'DeleteNotification');</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1385,14 +1379,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Pregled partnera', null, N'ReadPartner');</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1400,14 +1394,14 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih partnera', null, N'UpdatePartner');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Promena postojećih partnera', null, N'UpdatePartner');</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1415,14 +1409,14 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Dodavanje novih partnera', null, N'InsertPartner');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Dodavanje novih partnera', null, N'InsertPartner');</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1430,14 +1424,14 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje partnera', null, N'DeletePartner');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Brisanje partnera', null, N'DeletePartner');</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1445,14 +1439,14 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Pregled uloga', null, N'ReadRole');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Pregled uloga', null, N'ReadRole');</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1460,14 +1454,14 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Promena postojećih uloga', null, N'UpdateRole');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Promena postojećih uloga', null, N'UpdateRole');</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1475,14 +1469,14 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Dodavanje novih uloga', null, N'InsertRole');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Dodavanje novih uloga', null, N'InsertRole');</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1490,14 +1484,14 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Permissions(Name, Description, Code) values(N'Brisanje uloga', null, N'DeleteRole');</v>
+        <v>insert into Permission(Name, Description, Code) values(N'Brisanje uloga', null, N'DeleteRole');</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1562,21 +1556,21 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
@@ -1588,13 +1582,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', N'",C3,"', N'",D3,"');")</f>
@@ -1606,13 +1600,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', N'",C4,"', N'",D4,"');")</f>
@@ -1626,69 +1620,58 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
-        <v>delete from Genders; dbcc checkident (Genders, reseed, 0);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>delete from Gender; dbcc checkident (Gender, reseed, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,") values(N'",B3,"', N'",C3,"');")</f>
-        <v>insert into Genders(Name, NameLatin) values(N'Male', N'Muški');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B2,"');")</f>
+        <v>insert into Gender(Name) values(N'Name');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,") values(N'",B4,"', N'",C4,"');")</f>
-        <v>insert into Genders(Name, NameLatin) values(N'Female', N'Ženski');</v>
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
+        <v>insert into Gender(Name) values(N'Male');</v>
       </c>
     </row>
   </sheetData>
@@ -1713,15 +1696,15 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
@@ -1730,7 +1713,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
@@ -1739,7 +1722,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C67" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B4,"');")</f>
@@ -1748,7 +1731,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1757,7 +1740,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1766,7 +1749,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1775,7 +1758,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1784,7 +1767,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1793,7 +1776,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1802,7 +1785,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1811,7 +1794,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1820,7 +1803,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1829,7 +1812,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1838,7 +1821,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1847,7 +1830,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1856,7 +1839,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1865,7 +1848,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1874,7 +1857,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1883,7 +1866,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1892,7 +1875,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1901,7 +1884,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1910,7 +1893,7 @@
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1919,7 +1902,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1928,7 +1911,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1937,7 +1920,7 @@
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1946,7 +1929,7 @@
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1955,7 +1938,7 @@
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1964,7 +1947,7 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1973,7 +1956,7 @@
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1982,7 +1965,7 @@
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1991,7 +1974,7 @@
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2000,7 +1983,7 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2009,7 +1992,7 @@
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2018,7 +2001,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2027,7 +2010,7 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2036,7 +2019,7 @@
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2045,7 +2028,7 @@
     </row>
     <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2054,7 +2037,7 @@
     </row>
     <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2063,7 +2046,7 @@
     </row>
     <row r="40" spans="2:3">
       <c r="B40" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2072,7 +2055,7 @@
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2081,7 +2064,7 @@
     </row>
     <row r="42" spans="2:3">
       <c r="B42" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2090,7 +2073,7 @@
     </row>
     <row r="43" spans="2:3">
       <c r="B43" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2099,7 +2082,7 @@
     </row>
     <row r="44" spans="2:3">
       <c r="B44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2108,7 +2091,7 @@
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2117,7 +2100,7 @@
     </row>
     <row r="46" spans="2:3">
       <c r="B46" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2126,7 +2109,7 @@
     </row>
     <row r="47" spans="2:3">
       <c r="B47" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2135,7 +2118,7 @@
     </row>
     <row r="48" spans="2:3">
       <c r="B48" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2144,7 +2127,7 @@
     </row>
     <row r="49" spans="2:3">
       <c r="B49" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2153,7 +2136,7 @@
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2162,7 +2145,7 @@
     </row>
     <row r="51" spans="2:3">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2171,7 +2154,7 @@
     </row>
     <row r="52" spans="2:3">
       <c r="B52" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2180,7 +2163,7 @@
     </row>
     <row r="53" spans="2:3">
       <c r="B53" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2189,7 +2172,7 @@
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2198,7 +2181,7 @@
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2207,7 +2190,7 @@
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2216,7 +2199,7 @@
     </row>
     <row r="57" spans="2:3">
       <c r="B57" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2225,7 +2208,7 @@
     </row>
     <row r="58" spans="2:3">
       <c r="B58" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2234,7 +2217,7 @@
     </row>
     <row r="59" spans="2:3">
       <c r="B59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2243,7 +2226,7 @@
     </row>
     <row r="60" spans="2:3">
       <c r="B60" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2252,7 +2235,7 @@
     </row>
     <row r="61" spans="2:3">
       <c r="B61" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2261,7 +2244,7 @@
     </row>
     <row r="62" spans="2:3">
       <c r="B62" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2270,7 +2253,7 @@
     </row>
     <row r="63" spans="2:3">
       <c r="B63" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2279,7 +2262,7 @@
     </row>
     <row r="64" spans="2:3">
       <c r="B64" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2288,7 +2271,7 @@
     </row>
     <row r="65" spans="2:3">
       <c r="B65" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2297,7 +2280,7 @@
     </row>
     <row r="66" spans="2:3">
       <c r="B66" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2306,7 +2289,7 @@
     </row>
     <row r="67" spans="2:3">
       <c r="B67" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2315,7 +2298,7 @@
     </row>
     <row r="68" spans="2:3">
       <c r="B68" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C68" s="1" t="str">
         <f t="shared" ref="C68:C131" si="1">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B68,"');")</f>
@@ -2324,7 +2307,7 @@
     </row>
     <row r="69" spans="2:3">
       <c r="B69" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2333,7 +2316,7 @@
     </row>
     <row r="70" spans="2:3">
       <c r="B70" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2342,7 +2325,7 @@
     </row>
     <row r="71" spans="2:3">
       <c r="B71" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2351,7 +2334,7 @@
     </row>
     <row r="72" spans="2:3">
       <c r="B72" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2360,7 +2343,7 @@
     </row>
     <row r="73" spans="2:3">
       <c r="B73" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C73" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2369,7 +2352,7 @@
     </row>
     <row r="74" spans="2:3">
       <c r="B74" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C74" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2378,7 +2361,7 @@
     </row>
     <row r="75" spans="2:3">
       <c r="B75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2387,7 +2370,7 @@
     </row>
     <row r="76" spans="2:3">
       <c r="B76" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C76" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2396,7 +2379,7 @@
     </row>
     <row r="77" spans="2:3">
       <c r="B77" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C77" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2405,7 +2388,7 @@
     </row>
     <row r="78" spans="2:3">
       <c r="B78" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C78" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2414,7 +2397,7 @@
     </row>
     <row r="79" spans="2:3">
       <c r="B79" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C79" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2423,7 +2406,7 @@
     </row>
     <row r="80" spans="2:3">
       <c r="B80" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C80" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2432,7 +2415,7 @@
     </row>
     <row r="81" spans="2:3">
       <c r="B81" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C81" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2441,7 +2424,7 @@
     </row>
     <row r="82" spans="2:3">
       <c r="B82" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2450,7 +2433,7 @@
     </row>
     <row r="83" spans="2:3">
       <c r="B83" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C83" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2459,7 +2442,7 @@
     </row>
     <row r="84" spans="2:3">
       <c r="B84" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C84" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2468,7 +2451,7 @@
     </row>
     <row r="85" spans="2:3">
       <c r="B85" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C85" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2477,7 +2460,7 @@
     </row>
     <row r="86" spans="2:3">
       <c r="B86" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C86" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2486,7 +2469,7 @@
     </row>
     <row r="87" spans="2:3">
       <c r="B87" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C87" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2495,7 +2478,7 @@
     </row>
     <row r="88" spans="2:3">
       <c r="B88" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C88" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2504,7 +2487,7 @@
     </row>
     <row r="89" spans="2:3">
       <c r="B89" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C89" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2513,7 +2496,7 @@
     </row>
     <row r="90" spans="2:3">
       <c r="B90" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C90" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2522,7 +2505,7 @@
     </row>
     <row r="91" spans="2:3">
       <c r="B91" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C91" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2531,7 +2514,7 @@
     </row>
     <row r="92" spans="2:3">
       <c r="B92" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C92" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2540,7 +2523,7 @@
     </row>
     <row r="93" spans="2:3">
       <c r="B93" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C93" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2549,7 +2532,7 @@
     </row>
     <row r="94" spans="2:3">
       <c r="B94" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C94" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2558,7 +2541,7 @@
     </row>
     <row r="95" spans="2:3">
       <c r="B95" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C95" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2567,7 +2550,7 @@
     </row>
     <row r="96" spans="2:3">
       <c r="B96" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C96" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2576,7 +2559,7 @@
     </row>
     <row r="97" spans="2:3">
       <c r="B97" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C97" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2585,7 +2568,7 @@
     </row>
     <row r="98" spans="2:3">
       <c r="B98" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C98" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2594,7 +2577,7 @@
     </row>
     <row r="99" spans="2:3">
       <c r="B99" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C99" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2603,7 +2586,7 @@
     </row>
     <row r="100" spans="2:3">
       <c r="B100" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C100" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2612,7 +2595,7 @@
     </row>
     <row r="101" spans="2:3">
       <c r="B101" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C101" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2621,7 +2604,7 @@
     </row>
     <row r="102" spans="2:3">
       <c r="B102" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C102" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2630,7 +2613,7 @@
     </row>
     <row r="103" spans="2:3">
       <c r="B103" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C103" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2639,7 +2622,7 @@
     </row>
     <row r="104" spans="2:3">
       <c r="B104" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C104" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2648,7 +2631,7 @@
     </row>
     <row r="105" spans="2:3">
       <c r="B105" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C105" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2657,7 +2640,7 @@
     </row>
     <row r="106" spans="2:3">
       <c r="B106" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C106" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2666,7 +2649,7 @@
     </row>
     <row r="107" spans="2:3">
       <c r="B107" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C107" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2675,7 +2658,7 @@
     </row>
     <row r="108" spans="2:3">
       <c r="B108" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C108" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2684,7 +2667,7 @@
     </row>
     <row r="109" spans="2:3">
       <c r="B109" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C109" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2693,7 +2676,7 @@
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C110" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2702,7 +2685,7 @@
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C111" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2711,7 +2694,7 @@
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C112" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2720,7 +2703,7 @@
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C113" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2729,7 +2712,7 @@
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C114" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2738,7 +2721,7 @@
     </row>
     <row r="115" spans="2:3">
       <c r="B115" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C115" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2747,7 +2730,7 @@
     </row>
     <row r="116" spans="2:3">
       <c r="B116" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C116" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2756,7 +2739,7 @@
     </row>
     <row r="117" spans="2:3">
       <c r="B117" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C117" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2765,7 +2748,7 @@
     </row>
     <row r="118" spans="2:3">
       <c r="B118" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C118" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2774,7 +2757,7 @@
     </row>
     <row r="119" spans="2:3">
       <c r="B119" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C119" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2783,7 +2766,7 @@
     </row>
     <row r="120" spans="2:3">
       <c r="B120" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C120" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2792,7 +2775,7 @@
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C121" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2801,7 +2784,7 @@
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C122" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2810,7 +2793,7 @@
     </row>
     <row r="123" spans="2:3">
       <c r="B123" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C123" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2819,7 +2802,7 @@
     </row>
     <row r="124" spans="2:3">
       <c r="B124" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C124" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2828,7 +2811,7 @@
     </row>
     <row r="125" spans="2:3">
       <c r="B125" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C125" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2837,7 +2820,7 @@
     </row>
     <row r="126" spans="2:3">
       <c r="B126" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C126" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2846,7 +2829,7 @@
     </row>
     <row r="127" spans="2:3">
       <c r="B127" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C127" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2855,7 +2838,7 @@
     </row>
     <row r="128" spans="2:3">
       <c r="B128" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C128" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2864,7 +2847,7 @@
     </row>
     <row r="129" spans="2:3">
       <c r="B129" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C129" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2873,7 +2856,7 @@
     </row>
     <row r="130" spans="2:3">
       <c r="B130" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C130" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2882,7 +2865,7 @@
     </row>
     <row r="131" spans="2:3">
       <c r="B131" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C131" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2891,7 +2874,7 @@
     </row>
     <row r="132" spans="2:3">
       <c r="B132" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C132" s="1" t="str">
         <f t="shared" ref="C132:C177" si="2">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B132,"');")</f>
@@ -2900,7 +2883,7 @@
     </row>
     <row r="133" spans="2:3">
       <c r="B133" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C133" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2909,7 +2892,7 @@
     </row>
     <row r="134" spans="2:3">
       <c r="B134" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C134" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2918,7 +2901,7 @@
     </row>
     <row r="135" spans="2:3">
       <c r="B135" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C135" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2927,7 +2910,7 @@
     </row>
     <row r="136" spans="2:3">
       <c r="B136" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C136" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2936,7 +2919,7 @@
     </row>
     <row r="137" spans="2:3">
       <c r="B137" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C137" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2945,7 +2928,7 @@
     </row>
     <row r="138" spans="2:3">
       <c r="B138" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C138" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2954,7 +2937,7 @@
     </row>
     <row r="139" spans="2:3">
       <c r="B139" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C139" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2963,7 +2946,7 @@
     </row>
     <row r="140" spans="2:3">
       <c r="B140" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C140" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2972,7 +2955,7 @@
     </row>
     <row r="141" spans="2:3">
       <c r="B141" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C141" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2981,7 +2964,7 @@
     </row>
     <row r="142" spans="2:3">
       <c r="B142" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C142" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2990,7 +2973,7 @@
     </row>
     <row r="143" spans="2:3">
       <c r="B143" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C143" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2999,7 +2982,7 @@
     </row>
     <row r="144" spans="2:3">
       <c r="B144" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C144" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3008,7 +2991,7 @@
     </row>
     <row r="145" spans="2:3">
       <c r="B145" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C145" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3017,7 +3000,7 @@
     </row>
     <row r="146" spans="2:3">
       <c r="B146" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C146" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3026,7 +3009,7 @@
     </row>
     <row r="147" spans="2:3">
       <c r="B147" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C147" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3035,7 +3018,7 @@
     </row>
     <row r="148" spans="2:3">
       <c r="B148" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C148" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3044,7 +3027,7 @@
     </row>
     <row r="149" spans="2:3">
       <c r="B149" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C149" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3053,7 +3036,7 @@
     </row>
     <row r="150" spans="2:3">
       <c r="B150" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C150" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3062,7 +3045,7 @@
     </row>
     <row r="151" spans="2:3">
       <c r="B151" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C151" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3071,7 +3054,7 @@
     </row>
     <row r="152" spans="2:3">
       <c r="B152" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C152" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3080,7 +3063,7 @@
     </row>
     <row r="153" spans="2:3">
       <c r="B153" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C153" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3089,7 +3072,7 @@
     </row>
     <row r="154" spans="2:3">
       <c r="B154" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C154" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3098,7 +3081,7 @@
     </row>
     <row r="155" spans="2:3">
       <c r="B155" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C155" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3107,7 +3090,7 @@
     </row>
     <row r="156" spans="2:3">
       <c r="B156" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C156" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3116,7 +3099,7 @@
     </row>
     <row r="157" spans="2:3">
       <c r="B157" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C157" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3125,7 +3108,7 @@
     </row>
     <row r="158" spans="2:3">
       <c r="B158" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C158" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3134,7 +3117,7 @@
     </row>
     <row r="159" spans="2:3">
       <c r="B159" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C159" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3143,7 +3126,7 @@
     </row>
     <row r="160" spans="2:3">
       <c r="B160" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C160" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3152,7 +3135,7 @@
     </row>
     <row r="161" spans="2:3">
       <c r="B161" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C161" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3161,7 +3144,7 @@
     </row>
     <row r="162" spans="2:3">
       <c r="B162" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C162" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3170,7 +3153,7 @@
     </row>
     <row r="163" spans="2:3">
       <c r="B163" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C163" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3179,7 +3162,7 @@
     </row>
     <row r="164" spans="2:3">
       <c r="B164" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C164" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3188,7 +3171,7 @@
     </row>
     <row r="165" spans="2:3">
       <c r="B165" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C165" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3197,7 +3180,7 @@
     </row>
     <row r="166" spans="2:3">
       <c r="B166" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C166" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3206,7 +3189,7 @@
     </row>
     <row r="167" spans="2:3">
       <c r="B167" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C167" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3215,7 +3198,7 @@
     </row>
     <row r="168" spans="2:3">
       <c r="B168" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C168" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3224,7 +3207,7 @@
     </row>
     <row r="169" spans="2:3">
       <c r="B169" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C169" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3233,7 +3216,7 @@
     </row>
     <row r="170" spans="2:3">
       <c r="B170" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C170" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3242,7 +3225,7 @@
     </row>
     <row r="171" spans="2:3">
       <c r="B171" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C171" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3251,7 +3234,7 @@
     </row>
     <row r="172" spans="2:3">
       <c r="B172" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C172" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3260,7 +3243,7 @@
     </row>
     <row r="173" spans="2:3">
       <c r="B173" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C173" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3269,7 +3252,7 @@
     </row>
     <row r="174" spans="2:3">
       <c r="B174" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C174" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3278,7 +3261,7 @@
     </row>
     <row r="175" spans="2:3">
       <c r="B175" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C175" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3287,7 +3270,7 @@
     </row>
     <row r="176" spans="2:3">
       <c r="B176" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C176" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3296,7 +3279,7 @@
     </row>
     <row r="177" spans="2:3">
       <c r="B177" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C177" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3326,8 +3309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3341,21 +3324,21 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
@@ -3367,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="E3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', ",IF(TRIM(C3)&lt;&gt;"","N'"&amp;C3&amp;"'","null"),", N'",D3,"');")</f>
@@ -3386,10 +3369,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" ref="E4:E9" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
@@ -3405,10 +3388,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3424,10 +3407,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3443,10 +3426,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3462,10 +3445,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3481,10 +3464,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3500,10 +3483,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" ref="E10:E27" si="2">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B10,"', ",IF(TRIM(C10)&lt;&gt;"","N'"&amp;C10&amp;"'","null"),", N'",D10,"');")</f>
@@ -3519,10 +3502,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3538,10 +3521,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3557,10 +3540,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3576,10 +3559,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3595,10 +3578,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3614,10 +3597,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3633,10 +3616,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="2"/>
@@ -3652,10 +3635,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="2"/>
@@ -3671,10 +3654,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="2"/>
@@ -3690,10 +3673,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="2"/>
@@ -3709,10 +3692,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="2"/>
@@ -3728,10 +3711,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="2"/>
@@ -3747,10 +3730,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="2"/>
@@ -3766,10 +3749,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="2"/>
@@ -3785,10 +3768,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3804,10 +3787,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3823,10 +3806,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Working on the points history (achievements feature).
</commit_message>
<xml_diff>
--- a/Data/initialize-data.xlsx
+++ b/Data/initialize-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Municipalities" sheetId="5" r:id="rId5"/>
     <sheet name="Companies" sheetId="6" r:id="rId6"/>
     <sheet name="PartnerPermission" sheetId="7" r:id="rId7"/>
+    <sheet name="AchievementType" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="263">
   <si>
     <t>Name</t>
   </si>
@@ -91,12 +92,6 @@
     <t>DeleteNotification</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Municipalities</t>
   </si>
   <si>
@@ -797,6 +792,24 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>AchievementType</t>
+  </si>
+  <si>
+    <t>Transakcija</t>
+  </si>
+  <si>
+    <t>Muški</t>
+  </si>
+  <si>
+    <t>Ženski</t>
+  </si>
+  <si>
+    <t>Popunjavanje prvi put</t>
+  </si>
+  <si>
+    <t>Manuelno</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1261,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1274,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -1289,10 +1302,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" ref="E4:E17" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
@@ -1304,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -1334,10 +1347,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1349,7 +1362,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
@@ -1379,10 +1392,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1394,10 +1407,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1409,10 +1422,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1424,10 +1437,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1439,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -1454,10 +1467,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1469,7 +1482,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1484,7 +1497,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>7</v>
@@ -1622,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1634,7 +1647,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -1655,11 +1668,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>259</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B2,"');")</f>
-        <v>insert into Gender(Name) values(N'Name');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
+        <v>insert into Gender(Name) values(N'Muški');</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1667,11 +1680,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>260</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
-        <v>insert into Gender(Name) values(N'Male');</v>
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B4,"');")</f>
+        <v>insert into Gender(Name) values(N'Ženski');</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1709,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1713,7 +1726,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
@@ -1722,7 +1735,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C67" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B4,"');")</f>
@@ -1731,7 +1744,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1740,7 +1753,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1749,7 +1762,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1758,7 +1771,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1767,7 +1780,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1776,7 +1789,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1785,7 +1798,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1794,7 +1807,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1803,7 +1816,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1812,7 +1825,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1821,7 +1834,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1830,7 +1843,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1839,7 +1852,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1848,7 +1861,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1857,7 +1870,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1866,7 +1879,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1875,7 +1888,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1884,7 +1897,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1893,7 +1906,7 @@
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1902,7 +1915,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1911,7 +1924,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1920,7 +1933,7 @@
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1929,7 +1942,7 @@
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1938,7 +1951,7 @@
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1947,7 +1960,7 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1956,7 +1969,7 @@
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1965,7 +1978,7 @@
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1974,7 +1987,7 @@
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1983,7 +1996,7 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1992,7 +2005,7 @@
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2001,7 +2014,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2010,7 +2023,7 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2019,7 +2032,7 @@
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2028,7 +2041,7 @@
     </row>
     <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2037,7 +2050,7 @@
     </row>
     <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2046,7 +2059,7 @@
     </row>
     <row r="40" spans="2:3">
       <c r="B40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2055,7 +2068,7 @@
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2064,7 +2077,7 @@
     </row>
     <row r="42" spans="2:3">
       <c r="B42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2073,7 +2086,7 @@
     </row>
     <row r="43" spans="2:3">
       <c r="B43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2082,7 +2095,7 @@
     </row>
     <row r="44" spans="2:3">
       <c r="B44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2091,7 +2104,7 @@
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2100,7 +2113,7 @@
     </row>
     <row r="46" spans="2:3">
       <c r="B46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2109,7 +2122,7 @@
     </row>
     <row r="47" spans="2:3">
       <c r="B47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2118,7 +2131,7 @@
     </row>
     <row r="48" spans="2:3">
       <c r="B48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2127,7 +2140,7 @@
     </row>
     <row r="49" spans="2:3">
       <c r="B49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2136,7 +2149,7 @@
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2145,7 +2158,7 @@
     </row>
     <row r="51" spans="2:3">
       <c r="B51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2154,7 +2167,7 @@
     </row>
     <row r="52" spans="2:3">
       <c r="B52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2163,7 +2176,7 @@
     </row>
     <row r="53" spans="2:3">
       <c r="B53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2172,7 +2185,7 @@
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2181,7 +2194,7 @@
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2190,7 +2203,7 @@
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2199,7 +2212,7 @@
     </row>
     <row r="57" spans="2:3">
       <c r="B57" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2208,7 +2221,7 @@
     </row>
     <row r="58" spans="2:3">
       <c r="B58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2217,7 +2230,7 @@
     </row>
     <row r="59" spans="2:3">
       <c r="B59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2226,7 +2239,7 @@
     </row>
     <row r="60" spans="2:3">
       <c r="B60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2235,7 +2248,7 @@
     </row>
     <row r="61" spans="2:3">
       <c r="B61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2244,7 +2257,7 @@
     </row>
     <row r="62" spans="2:3">
       <c r="B62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2253,7 +2266,7 @@
     </row>
     <row r="63" spans="2:3">
       <c r="B63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2262,7 +2275,7 @@
     </row>
     <row r="64" spans="2:3">
       <c r="B64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2271,7 +2284,7 @@
     </row>
     <row r="65" spans="2:3">
       <c r="B65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2280,7 +2293,7 @@
     </row>
     <row r="66" spans="2:3">
       <c r="B66" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2289,7 +2302,7 @@
     </row>
     <row r="67" spans="2:3">
       <c r="B67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2298,7 +2311,7 @@
     </row>
     <row r="68" spans="2:3">
       <c r="B68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C68" s="1" t="str">
         <f t="shared" ref="C68:C131" si="1">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B68,"');")</f>
@@ -2307,7 +2320,7 @@
     </row>
     <row r="69" spans="2:3">
       <c r="B69" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2316,7 +2329,7 @@
     </row>
     <row r="70" spans="2:3">
       <c r="B70" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2325,7 +2338,7 @@
     </row>
     <row r="71" spans="2:3">
       <c r="B71" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2334,7 +2347,7 @@
     </row>
     <row r="72" spans="2:3">
       <c r="B72" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2343,7 +2356,7 @@
     </row>
     <row r="73" spans="2:3">
       <c r="B73" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C73" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2352,7 +2365,7 @@
     </row>
     <row r="74" spans="2:3">
       <c r="B74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C74" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2361,7 +2374,7 @@
     </row>
     <row r="75" spans="2:3">
       <c r="B75" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2370,7 +2383,7 @@
     </row>
     <row r="76" spans="2:3">
       <c r="B76" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C76" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2379,7 +2392,7 @@
     </row>
     <row r="77" spans="2:3">
       <c r="B77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C77" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2388,7 +2401,7 @@
     </row>
     <row r="78" spans="2:3">
       <c r="B78" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C78" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2397,7 +2410,7 @@
     </row>
     <row r="79" spans="2:3">
       <c r="B79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C79" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2406,7 +2419,7 @@
     </row>
     <row r="80" spans="2:3">
       <c r="B80" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C80" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2415,7 +2428,7 @@
     </row>
     <row r="81" spans="2:3">
       <c r="B81" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C81" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2424,7 +2437,7 @@
     </row>
     <row r="82" spans="2:3">
       <c r="B82" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2433,7 +2446,7 @@
     </row>
     <row r="83" spans="2:3">
       <c r="B83" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C83" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2442,7 +2455,7 @@
     </row>
     <row r="84" spans="2:3">
       <c r="B84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C84" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2451,7 +2464,7 @@
     </row>
     <row r="85" spans="2:3">
       <c r="B85" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C85" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2460,7 +2473,7 @@
     </row>
     <row r="86" spans="2:3">
       <c r="B86" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C86" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2469,7 +2482,7 @@
     </row>
     <row r="87" spans="2:3">
       <c r="B87" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C87" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2478,7 +2491,7 @@
     </row>
     <row r="88" spans="2:3">
       <c r="B88" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2487,7 +2500,7 @@
     </row>
     <row r="89" spans="2:3">
       <c r="B89" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C89" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2496,7 +2509,7 @@
     </row>
     <row r="90" spans="2:3">
       <c r="B90" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C90" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2505,7 +2518,7 @@
     </row>
     <row r="91" spans="2:3">
       <c r="B91" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C91" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2514,7 +2527,7 @@
     </row>
     <row r="92" spans="2:3">
       <c r="B92" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C92" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2523,7 +2536,7 @@
     </row>
     <row r="93" spans="2:3">
       <c r="B93" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C93" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2532,7 +2545,7 @@
     </row>
     <row r="94" spans="2:3">
       <c r="B94" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C94" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2541,7 +2554,7 @@
     </row>
     <row r="95" spans="2:3">
       <c r="B95" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C95" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2550,7 +2563,7 @@
     </row>
     <row r="96" spans="2:3">
       <c r="B96" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C96" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2559,7 +2572,7 @@
     </row>
     <row r="97" spans="2:3">
       <c r="B97" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C97" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2568,7 +2581,7 @@
     </row>
     <row r="98" spans="2:3">
       <c r="B98" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C98" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2577,7 +2590,7 @@
     </row>
     <row r="99" spans="2:3">
       <c r="B99" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C99" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2586,7 +2599,7 @@
     </row>
     <row r="100" spans="2:3">
       <c r="B100" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C100" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2595,7 +2608,7 @@
     </row>
     <row r="101" spans="2:3">
       <c r="B101" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C101" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2604,7 +2617,7 @@
     </row>
     <row r="102" spans="2:3">
       <c r="B102" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C102" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2613,7 +2626,7 @@
     </row>
     <row r="103" spans="2:3">
       <c r="B103" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C103" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2622,7 +2635,7 @@
     </row>
     <row r="104" spans="2:3">
       <c r="B104" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C104" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2631,7 +2644,7 @@
     </row>
     <row r="105" spans="2:3">
       <c r="B105" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C105" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2640,7 +2653,7 @@
     </row>
     <row r="106" spans="2:3">
       <c r="B106" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C106" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2649,7 +2662,7 @@
     </row>
     <row r="107" spans="2:3">
       <c r="B107" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C107" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2658,7 +2671,7 @@
     </row>
     <row r="108" spans="2:3">
       <c r="B108" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C108" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2667,7 +2680,7 @@
     </row>
     <row r="109" spans="2:3">
       <c r="B109" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C109" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2676,7 +2689,7 @@
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C110" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2685,7 +2698,7 @@
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C111" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2694,7 +2707,7 @@
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C112" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2703,7 +2716,7 @@
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C113" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2712,7 +2725,7 @@
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C114" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2721,7 +2734,7 @@
     </row>
     <row r="115" spans="2:3">
       <c r="B115" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C115" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2730,7 +2743,7 @@
     </row>
     <row r="116" spans="2:3">
       <c r="B116" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C116" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2739,7 +2752,7 @@
     </row>
     <row r="117" spans="2:3">
       <c r="B117" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C117" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2748,7 +2761,7 @@
     </row>
     <row r="118" spans="2:3">
       <c r="B118" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C118" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2757,7 +2770,7 @@
     </row>
     <row r="119" spans="2:3">
       <c r="B119" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C119" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2766,7 +2779,7 @@
     </row>
     <row r="120" spans="2:3">
       <c r="B120" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C120" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2775,7 +2788,7 @@
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C121" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2784,7 +2797,7 @@
     </row>
     <row r="122" spans="2:3">
       <c r="B122" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C122" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2793,7 +2806,7 @@
     </row>
     <row r="123" spans="2:3">
       <c r="B123" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C123" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2802,7 +2815,7 @@
     </row>
     <row r="124" spans="2:3">
       <c r="B124" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C124" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2811,7 +2824,7 @@
     </row>
     <row r="125" spans="2:3">
       <c r="B125" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C125" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2820,7 +2833,7 @@
     </row>
     <row r="126" spans="2:3">
       <c r="B126" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C126" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2829,7 +2842,7 @@
     </row>
     <row r="127" spans="2:3">
       <c r="B127" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C127" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2838,7 +2851,7 @@
     </row>
     <row r="128" spans="2:3">
       <c r="B128" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C128" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2847,7 +2860,7 @@
     </row>
     <row r="129" spans="2:3">
       <c r="B129" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C129" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2856,7 +2869,7 @@
     </row>
     <row r="130" spans="2:3">
       <c r="B130" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C130" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2865,7 +2878,7 @@
     </row>
     <row r="131" spans="2:3">
       <c r="B131" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C131" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2874,7 +2887,7 @@
     </row>
     <row r="132" spans="2:3">
       <c r="B132" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C132" s="1" t="str">
         <f t="shared" ref="C132:C177" si="2">CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B132,"');")</f>
@@ -2883,7 +2896,7 @@
     </row>
     <row r="133" spans="2:3">
       <c r="B133" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C133" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2892,7 +2905,7 @@
     </row>
     <row r="134" spans="2:3">
       <c r="B134" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C134" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2901,7 +2914,7 @@
     </row>
     <row r="135" spans="2:3">
       <c r="B135" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C135" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2910,7 +2923,7 @@
     </row>
     <row r="136" spans="2:3">
       <c r="B136" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C136" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2919,7 +2932,7 @@
     </row>
     <row r="137" spans="2:3">
       <c r="B137" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C137" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2928,7 +2941,7 @@
     </row>
     <row r="138" spans="2:3">
       <c r="B138" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C138" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2937,7 +2950,7 @@
     </row>
     <row r="139" spans="2:3">
       <c r="B139" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C139" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2946,7 +2959,7 @@
     </row>
     <row r="140" spans="2:3">
       <c r="B140" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C140" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2955,7 +2968,7 @@
     </row>
     <row r="141" spans="2:3">
       <c r="B141" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C141" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2964,7 +2977,7 @@
     </row>
     <row r="142" spans="2:3">
       <c r="B142" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C142" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2973,7 +2986,7 @@
     </row>
     <row r="143" spans="2:3">
       <c r="B143" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C143" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2982,7 +2995,7 @@
     </row>
     <row r="144" spans="2:3">
       <c r="B144" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C144" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2991,7 +3004,7 @@
     </row>
     <row r="145" spans="2:3">
       <c r="B145" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C145" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3000,7 +3013,7 @@
     </row>
     <row r="146" spans="2:3">
       <c r="B146" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C146" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3009,7 +3022,7 @@
     </row>
     <row r="147" spans="2:3">
       <c r="B147" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C147" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3018,7 +3031,7 @@
     </row>
     <row r="148" spans="2:3">
       <c r="B148" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C148" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3027,7 +3040,7 @@
     </row>
     <row r="149" spans="2:3">
       <c r="B149" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C149" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3036,7 +3049,7 @@
     </row>
     <row r="150" spans="2:3">
       <c r="B150" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C150" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3045,7 +3058,7 @@
     </row>
     <row r="151" spans="2:3">
       <c r="B151" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C151" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3054,7 +3067,7 @@
     </row>
     <row r="152" spans="2:3">
       <c r="B152" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C152" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3063,7 +3076,7 @@
     </row>
     <row r="153" spans="2:3">
       <c r="B153" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C153" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3072,7 +3085,7 @@
     </row>
     <row r="154" spans="2:3">
       <c r="B154" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C154" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3081,7 +3094,7 @@
     </row>
     <row r="155" spans="2:3">
       <c r="B155" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C155" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3090,7 +3103,7 @@
     </row>
     <row r="156" spans="2:3">
       <c r="B156" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C156" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3099,7 +3112,7 @@
     </row>
     <row r="157" spans="2:3">
       <c r="B157" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C157" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3108,7 +3121,7 @@
     </row>
     <row r="158" spans="2:3">
       <c r="B158" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C158" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3117,7 +3130,7 @@
     </row>
     <row r="159" spans="2:3">
       <c r="B159" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C159" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3126,7 +3139,7 @@
     </row>
     <row r="160" spans="2:3">
       <c r="B160" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C160" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3135,7 +3148,7 @@
     </row>
     <row r="161" spans="2:3">
       <c r="B161" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C161" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3144,7 +3157,7 @@
     </row>
     <row r="162" spans="2:3">
       <c r="B162" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C162" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3153,7 +3166,7 @@
     </row>
     <row r="163" spans="2:3">
       <c r="B163" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C163" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3162,7 +3175,7 @@
     </row>
     <row r="164" spans="2:3">
       <c r="B164" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C164" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3171,7 +3184,7 @@
     </row>
     <row r="165" spans="2:3">
       <c r="B165" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C165" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3180,7 +3193,7 @@
     </row>
     <row r="166" spans="2:3">
       <c r="B166" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C166" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3189,7 +3202,7 @@
     </row>
     <row r="167" spans="2:3">
       <c r="B167" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C167" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3198,7 +3211,7 @@
     </row>
     <row r="168" spans="2:3">
       <c r="B168" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C168" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3207,7 +3220,7 @@
     </row>
     <row r="169" spans="2:3">
       <c r="B169" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C169" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3216,7 +3229,7 @@
     </row>
     <row r="170" spans="2:3">
       <c r="B170" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C170" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3225,7 +3238,7 @@
     </row>
     <row r="171" spans="2:3">
       <c r="B171" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C171" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3234,7 +3247,7 @@
     </row>
     <row r="172" spans="2:3">
       <c r="B172" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C172" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3243,7 +3256,7 @@
     </row>
     <row r="173" spans="2:3">
       <c r="B173" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C173" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3252,7 +3265,7 @@
     </row>
     <row r="174" spans="2:3">
       <c r="B174" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C174" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3261,7 +3274,7 @@
     </row>
     <row r="175" spans="2:3">
       <c r="B175" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C175" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3270,7 +3283,7 @@
     </row>
     <row r="176" spans="2:3">
       <c r="B176" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C176" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3279,7 +3292,7 @@
     </row>
     <row r="177" spans="2:3">
       <c r="B177" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C177" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3324,7 +3337,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -3350,10 +3363,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E3" t="str">
         <f>CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B3,"', ",IF(TRIM(C3)&lt;&gt;"","N'"&amp;C3&amp;"'","null"),", N'",D3,"');")</f>
@@ -3369,10 +3382,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" ref="E4:E9" si="0">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B4,"', ",IF(TRIM(C4)&lt;&gt;"","N'"&amp;C4&amp;"'","null"),", N'",D4,"');")</f>
@@ -3388,10 +3401,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3407,10 +3420,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3426,10 +3439,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3445,10 +3458,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3464,10 +3477,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3486,7 +3499,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" ref="E10:E27" si="2">CONCATENATE("insert into ",$A$1,"(",$B$2,", ",$C$2,", ",$D$2,") values(N'",B10,"', ",IF(TRIM(C10)&lt;&gt;"","N'"&amp;C10&amp;"'","null"),", N'",D10,"');")</f>
@@ -3502,10 +3515,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3521,10 +3534,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3543,7 +3556,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3559,10 +3572,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3578,10 +3591,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3597,7 +3610,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>
@@ -3616,10 +3629,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="2"/>
@@ -3635,7 +3648,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
@@ -3654,7 +3667,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -3673,10 +3686,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="2"/>
@@ -3692,10 +3705,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="2"/>
@@ -3711,10 +3724,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="2"/>
@@ -3730,10 +3743,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="2"/>
@@ -3749,10 +3762,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="2"/>
@@ -3768,10 +3781,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3787,10 +3800,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3806,10 +3819,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3818,6 +3831,79 @@
       <c r="R27" s="1" t="str">
         <f t="shared" si="3"/>
         <v>DeleteBusinessSystem = 25,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>CONCATENATE("delete from ",$A$1,"; dbcc checkident (",$A$1,", reseed, 0);")</f>
+        <v>delete from AchievementType; dbcc checkident (AchievementType, reseed, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B3,"');")</f>
+        <v>insert into AchievementType(Name) values(N'Transakcija');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B4,"');")</f>
+        <v>insert into AchievementType(Name) values(N'Popunjavanje prvi put');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>CONCATENATE("insert into ",$A$1,"(",$B$2,") values(N'",B5,"');")</f>
+        <v>insert into AchievementType(Name) values(N'Manuelno');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>